<commit_message>
Introduction 04.12.2024 (Species and study site)
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5C994D-C850-3949-9E76-96CC2E21B9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA9A52B-2414-AE48-8164-674BA9CAB980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48680" yWindow="680" windowWidth="18960" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="14800" yWindow="900" windowWidth="14440" windowHeight="16880" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
   <si>
     <t>Paper Title</t>
   </si>
@@ -406,6 +406,45 @@
       </rPr>
       <t>residual within individual variance</t>
     </r>
+  </si>
+  <si>
+    <t>Vernal behaviour of the yellow-bellied marmot</t>
+  </si>
+  <si>
+    <t>Anim. Behav.</t>
+  </si>
+  <si>
+    <t>YELLOWSTONE POPULATION</t>
+  </si>
+  <si>
+    <t>Reproductive and agonistic behaviour in the first 5 weeks post-hibernation</t>
+  </si>
+  <si>
+    <t>behavioral observation in natural conditions</t>
+  </si>
+  <si>
+    <t>Yellow-bellied marmots (Marmota flaviventris) hibernate socially</t>
+  </si>
+  <si>
+    <t>J. Mamm.</t>
+  </si>
+  <si>
+    <t>Blumstein, Nicodemus and Zugmeyer</t>
+  </si>
+  <si>
+    <t>Social effects on emergence from hibernation in yellow-bellied marmots</t>
+  </si>
+  <si>
+    <t>Blumstein</t>
+  </si>
+  <si>
+    <t> Yellow-bellied marmots do not compensate for a late start: the role of maternal investment in shaping life-history trajectories</t>
+  </si>
+  <si>
+    <t>Evolutionary Ecology</t>
+  </si>
+  <si>
+    <t>Monclus, Pang, Blumstein</t>
   </si>
 </sst>
 </file>
@@ -699,7 +738,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -789,15 +828,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1136,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,7 +1258,7 @@
       <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="2" t="s">
@@ -1363,7 +1398,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1644,7 +1679,7 @@
       <c r="D15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="34" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="10" t="s">
@@ -1746,7 +1781,7 @@
       <c r="J18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="36" t="s">
+      <c r="K18" s="8" t="s">
         <v>12</v>
       </c>
       <c r="L18" s="2"/>
@@ -1755,41 +1790,83 @@
       </c>
       <c r="N18" s="15">
         <f>N19+N25</f>
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="7"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="A19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1965</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="M19" s="16" t="s">
         <v>9</v>
       </c>
       <c r="N19" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="8"/>
-      <c r="F20" s="4"/>
+      <c r="A20" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2004</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="G20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="M20" s="17" t="s">
         <v>15</v>
       </c>
       <c r="N20" s="18">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>16</v>
@@ -1800,36 +1877,68 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="M21" s="21" t="s">
         <v>17</v>
       </c>
       <c r="N21" s="22">
         <f>COUNTIF(F:F, "no")</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="F22" s="9"/>
+      <c r="A22" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
+      <c r="I22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
@@ -1845,7 +1954,7 @@
       </c>
       <c r="N23" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2578,6 +2687,9 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B2058B0C-BE95-DA4B-8AE3-AB82AA4C9E64}"/>
     <hyperlink ref="A14" r:id="rId2" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Ozgul_etal_Nature_2010_all.pdf" xr:uid="{C5D55BD9-EC2E-9A4A-91B8-D261357FED7A}"/>
+    <hyperlink ref="A20" r:id="rId3" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Blumstein_etal_2004_JM.pdf" xr:uid="{3A8C16DB-3B31-5A4F-8393-AE03B214C5D1}"/>
+    <hyperlink ref="A21" r:id="rId4" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Blumstein_2009_JM.pdf" xr:uid="{25712E07-C75B-EE4C-A484-0AB3BB020C76}"/>
+    <hyperlink ref="A22" r:id="rId5" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Monclus_etal_2014_EvolEcol.pdf" xr:uid="{5C5293D3-C93C-8049-99C4-7FAB32E99F55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Introduction - plasticity vs evol; LHT and resp to climate change, I*E bet-hedging - 05.12.2024
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA9A52B-2414-AE48-8164-674BA9CAB980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A18945D-C3CC-FD4D-A592-F92A3B79B57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14800" yWindow="900" windowWidth="14440" windowHeight="16880" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="115">
   <si>
     <t>Paper Title</t>
   </si>
@@ -445,6 +445,57 @@
   </si>
   <si>
     <t>Monclus, Pang, Blumstein</t>
+  </si>
+  <si>
+    <t>Probing variation in reaction norms in wild populations: the importance of reliable environmental proxies</t>
+  </si>
+  <si>
+    <t>Oikos</t>
+  </si>
+  <si>
+    <t>Ramakers, Reed, Harris, Gienapp</t>
+  </si>
+  <si>
+    <r>
+      <t>Importance of the environmental proxies to detect slope variation in reaction norm (so I * E and G * E) =&gt; Environment Specific Mean phenotype (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ESM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>The Origin of Species: By Means of Natural Selection, or the Preservation of Favoured Races in the Struggle for Life</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>Evolution by natural selection</t>
+  </si>
+  <si>
+    <t>Costs and limits of phenotypic plasticity</t>
+  </si>
+  <si>
+    <t>DeWitt, Sih &amp; Wilson</t>
+  </si>
+  <si>
+    <t>Limits and costs of the plasticity</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1223,7 @@
   <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,7 +1769,9 @@
       <c r="G16" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J16" s="7" t="s">
         <v>12</v>
       </c>
@@ -1790,7 +1843,7 @@
       </c>
       <c r="N18" s="15">
         <f>N19+N25</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1832,7 +1885,7 @@
       </c>
       <c r="N19" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1866,7 +1919,7 @@
       </c>
       <c r="N20" s="18">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>16</v>
@@ -1909,7 +1962,7 @@
       </c>
       <c r="N21" s="22">
         <f>COUNTIF(F:F, "no")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1943,41 +1996,103 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="M23" s="23" t="s">
         <v>10</v>
       </c>
       <c r="N23" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="12"/>
+      <c r="A24" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1859</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="I24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="A25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1998</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="L25" s="8"/>
       <c r="M25" s="23" t="s">
         <v>18</v>
@@ -2692,5 +2807,6 @@
     <hyperlink ref="A22" r:id="rId5" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Monclus_etal_2014_EvolEcol.pdf" xr:uid="{5C5293D3-C93C-8049-99C4-7FAB32E99F55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Introduction - Global warming and body mass; QG and animal models - 05.12.2024
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A18945D-C3CC-FD4D-A592-F92A3B79B57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE3C959-F193-584F-BC04-6EA76AF7CDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14800" yWindow="900" windowWidth="14440" windowHeight="16880" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="122">
   <si>
     <t>Paper Title</t>
   </si>
@@ -496,6 +496,27 @@
   </si>
   <si>
     <t>Limits and costs of the plasticity</t>
+  </si>
+  <si>
+    <t>The study of quantitative genetics in wild populations</t>
+  </si>
+  <si>
+    <t>Oxford university press</t>
+  </si>
+  <si>
+    <t>Kruuk, Charmantier &amp; Garant</t>
+  </si>
+  <si>
+    <t>General quantitative genetics</t>
+  </si>
+  <si>
+    <t>Genetics and Analysis of Quantitative Traits</t>
+  </si>
+  <si>
+    <t>Sinauer</t>
+  </si>
+  <si>
+    <t>Lynch &amp; Walsh</t>
   </si>
 </sst>
 </file>
@@ -1220,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1449,24 +1470,26 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
+      <c r="A7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="C7" s="2">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>35</v>
+        <v>117</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
@@ -1478,133 +1501,130 @@
       <c r="K7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2009</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>2011</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="F10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="10" t="s">
+      <c r="I10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>2010</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="F11" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2023</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1618,27 +1638,27 @@
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2">
-        <v>2004</v>
+        <v>2023</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>57</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1652,26 +1672,26 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>12</v>
@@ -1686,28 +1706,26 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>67</v>
+        <v>60</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>12</v>
@@ -1715,274 +1733,275 @@
       <c r="J14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="K14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2">
         <v>1992</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E16" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="5" t="s">
+      <c r="I16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="K16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <v>2011</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="12" t="s">
+      <c r="F17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
+      <c r="I17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="2">
         <v>2008</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="F18" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+      <c r="I18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <v>2015</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="14" t="s">
+      <c r="I19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="N18" s="15">
-        <f>N19+N25</f>
+      <c r="N19" s="15">
+        <f>N20+N26</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1965</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="8">
-        <v>1965</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="F20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" s="16" t="s">
+      <c r="I20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C21" s="2">
         <v>2004</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="I20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20" s="17" t="s">
+      <c r="G21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N20" s="18">
+      <c r="N21" s="18">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>15</v>
-      </c>
-      <c r="O20" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="P20" s="20">
+      <c r="O21" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" s="20">
         <f>COUNTIF(E:E, "Software/Package")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="2">
-        <v>2009</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M21" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" s="22">
-        <f>COUNTIF(F:F, "no")</f>
-        <v>8</v>
-      </c>
-    </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C22" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>104</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E22" s="2"/>
       <c r="F22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1992,188 +2011,228 @@
       <c r="K22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
+      <c r="M22" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="22">
+        <f>COUNTIF(F:F, "no")</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <v>2023</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="F24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M23" s="23" t="s">
+      <c r="I24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="N23" s="20">
+      <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>1859</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G25" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C26" s="2">
         <v>1998</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="2" t="s">
+      <c r="F26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="8"/>
-      <c r="M25" s="23" t="s">
+      <c r="I26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="8"/>
+      <c r="M26" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="N25" s="20">
+      <c r="N26" s="20">
         <f>COUNTIF(J:J, "no")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="L26" s="2"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="F27" s="10"/>
-      <c r="J27" s="2"/>
+      <c r="A27" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1998</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
+      <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="8"/>
-      <c r="G28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="F28" s="10"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="2"/>
+      <c r="D29" s="8"/>
+      <c r="G29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="8"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
+      <c r="E30" s="2"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="2"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
       <c r="F32" s="25"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="2"/>
+      <c r="G32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="7"/>
+      <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
@@ -2186,7 +2245,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="K33" s="7"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
@@ -2200,86 +2259,85 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="8"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="13"/>
+      <c r="E35" s="2"/>
       <c r="F35" s="25"/>
       <c r="G35" s="12"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
+      <c r="L35" s="8"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="8"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="2"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="24"/>
-      <c r="B37" s="2"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="8"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="8"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="12"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="2"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="G39" s="12"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="2"/>
+      <c r="J39" s="7"/>
       <c r="K39" s="7"/>
+      <c r="L39" s="8"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="F40" s="10"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="7"/>
       <c r="J40" s="2"/>
+      <c r="K40" s="7"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="F41" s="10"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
@@ -2287,7 +2345,7 @@
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="10"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="12"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -2296,60 +2354,62 @@
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="8"/>
+      <c r="E43" s="2"/>
       <c r="F43" s="10"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="E44" s="8"/>
       <c r="F44" s="10"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
       <c r="F45" s="10"/>
-      <c r="J45" s="7"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="8"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
+      <c r="F46" s="10"/>
       <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="8"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
       <c r="F47" s="9"/>
       <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
@@ -2362,7 +2422,6 @@
       <c r="E48" s="2"/>
       <c r="F48" s="9"/>
       <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
@@ -2379,7 +2438,6 @@
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
-      <c r="L49" s="2"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
@@ -2393,16 +2451,19 @@
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
+      <c r="L50" s="2"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
-      <c r="B51" s="2"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="27"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2410,122 +2471,120 @@
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="27"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
+      <c r="K52" s="7"/>
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
+      <c r="A53" s="3"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="8"/>
       <c r="F53" s="25"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="8"/>
+      <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
-      <c r="K53" s="7"/>
+      <c r="K53" s="2"/>
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="28"/>
+      <c r="A54" s="6"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
+      <c r="E54" s="8"/>
       <c r="F54" s="25"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="8"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
+      <c r="K54" s="7"/>
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="10"/>
+      <c r="F55" s="25"/>
       <c r="G55" s="12"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="6"/>
-      <c r="B57" s="2"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="8"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="7"/>
       <c r="F57" s="29"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
       <c r="K57" s="7"/>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
+      <c r="A58" s="6"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="4"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="29"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
+      <c r="H58" s="8"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
+      <c r="K58" s="7"/>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="11"/>
+      <c r="A59" s="3"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="29"/>
-      <c r="G59" s="12"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="24"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="2"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="12"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="11"/>
-      <c r="B61" s="2"/>
+      <c r="A61" s="24"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="29"/>
-      <c r="G61" s="12"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -2545,27 +2604,29 @@
       <c r="K62" s="2"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="6"/>
-      <c r="B63" s="8"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="7"/>
+      <c r="E63" s="2"/>
       <c r="F63" s="29"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
-      <c r="B64" s="2"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="30"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="29"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
       <c r="K64" s="7"/>
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2573,13 +2634,11 @@
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="30"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
+      <c r="K65" s="7"/>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
@@ -2621,26 +2680,26 @@
       <c r="K68" s="2"/>
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="11"/>
+      <c r="A69" s="3"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="12"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
+      <c r="A70" s="11"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="12"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
@@ -2652,7 +2711,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="13"/>
-      <c r="F71" s="25"/>
+      <c r="F71" s="4"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -2665,7 +2724,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="13"/>
-      <c r="F72" s="4"/>
+      <c r="F72" s="25"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -2690,7 +2749,8 @@
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
-      <c r="F74" s="25"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="4"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -2702,10 +2762,12 @@
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
-      <c r="F75" s="10"/>
+      <c r="F75" s="25"/>
       <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
@@ -2723,27 +2785,26 @@
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="F77" s="10"/>
+      <c r="G77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
-      <c r="D78" s="31"/>
+      <c r="D78" s="2"/>
       <c r="F78" s="10"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
     <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="32"/>
+      <c r="A79" s="3"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="D79" s="31"/>
       <c r="F79" s="10"/>
-      <c r="G79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
@@ -2754,12 +2815,13 @@
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="F80" s="10"/>
+      <c r="G80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="24"/>
+      <c r="A81" s="32"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -2779,7 +2841,7 @@
       <c r="K82" s="2"/>
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="32"/>
+      <c r="A83" s="24"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -2788,7 +2850,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="32"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2798,13 +2860,23 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="32"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="F85" s="10"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B2058B0C-BE95-DA4B-8AE3-AB82AA4C9E64}"/>
-    <hyperlink ref="A14" r:id="rId2" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Ozgul_etal_Nature_2010_all.pdf" xr:uid="{C5D55BD9-EC2E-9A4A-91B8-D261357FED7A}"/>
-    <hyperlink ref="A20" r:id="rId3" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Blumstein_etal_2004_JM.pdf" xr:uid="{3A8C16DB-3B31-5A4F-8393-AE03B214C5D1}"/>
-    <hyperlink ref="A21" r:id="rId4" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Blumstein_2009_JM.pdf" xr:uid="{25712E07-C75B-EE4C-A484-0AB3BB020C76}"/>
-    <hyperlink ref="A22" r:id="rId5" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Monclus_etal_2014_EvolEcol.pdf" xr:uid="{5C5293D3-C93C-8049-99C4-7FAB32E99F55}"/>
+    <hyperlink ref="A15" r:id="rId2" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Ozgul_etal_Nature_2010_all.pdf" xr:uid="{C5D55BD9-EC2E-9A4A-91B8-D261357FED7A}"/>
+    <hyperlink ref="A21" r:id="rId3" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Blumstein_etal_2004_JM.pdf" xr:uid="{3A8C16DB-3B31-5A4F-8393-AE03B214C5D1}"/>
+    <hyperlink ref="A22" r:id="rId4" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Blumstein_2009_JM.pdf" xr:uid="{25712E07-C75B-EE4C-A484-0AB3BB020C76}"/>
+    <hyperlink ref="A23" r:id="rId5" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Monclus_etal_2014_EvolEcol.pdf" xr:uid="{5C5293D3-C93C-8049-99C4-7FAB32E99F55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
return from vacation: review until "link with hibernation" (included) - still need to write the first part (C.C) tho
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451968A9-5A22-E342-A467-554455001BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F13C3F-A3A1-EE4E-948F-C28A3D11AECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29240" windowHeight="16860" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="176">
   <si>
     <t>Paper Title</t>
   </si>
@@ -622,6 +622,63 @@
   </si>
   <si>
     <t>ggplot2</t>
+  </si>
+  <si>
+    <t>Precipitation and Temperature Trends and Cycles Derived from Historical 1890-2019 Weather Data for the City of Ottawa, Ontario, Canada</t>
+  </si>
+  <si>
+    <t>Environments</t>
+  </si>
+  <si>
+    <t>Walsh &amp; Patterson</t>
+  </si>
+  <si>
+    <t>Cimatic trend in the last century in Ottawa</t>
+  </si>
+  <si>
+    <t>Future projections of temperature changes in Ottawa, Canada through stepwise clustered downscaling of multiple GCMs under RCPs</t>
+  </si>
+  <si>
+    <t>Climate Dynamics</t>
+  </si>
+  <si>
+    <t>Zhai, Huang, Wang, Zhou, Lu, Li</t>
+  </si>
+  <si>
+    <t>Climate projections for Ottawa</t>
+  </si>
+  <si>
+    <t>Hibernation</t>
+  </si>
+  <si>
+    <t>Current biology</t>
+  </si>
+  <si>
+    <t>Geiser</t>
+  </si>
+  <si>
+    <t>Hibernation' definition</t>
+  </si>
+  <si>
+    <t>Mammalian hibernation</t>
+  </si>
+  <si>
+    <t>Phil. Trans. R. Soc. Lond. B</t>
+  </si>
+  <si>
+    <t>Nedergaard &amp; Cannon</t>
+  </si>
+  <si>
+    <t>Climate and the match or mismatch between predator requirements and resource availability</t>
+  </si>
+  <si>
+    <t>Durant, Hjermann, Ottersen, Stenseth</t>
+  </si>
+  <si>
+    <t>Clim. Res.</t>
+  </si>
+  <si>
+    <t>changes in phenology as a universal response to climate change</t>
   </si>
 </sst>
 </file>
@@ -1351,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2005,7 +2062,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2047,7 +2104,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2124,7 +2181,7 @@
       </c>
       <c r="N22" s="22">
         <f>COUNTIF(F:F, "no")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2190,7 +2247,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2581,56 +2638,152 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
+      <c r="A37" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2022</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="8"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="A38" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="2"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="12"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
+      <c r="A39" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="L39" s="8"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="2"/>
+      <c r="A40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1990</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="7"/>
+      <c r="I40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="F41" s="10"/>
-      <c r="J41" s="2"/>
+      <c r="A41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
@@ -2639,7 +2792,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="26"/>
-      <c r="G42" s="12"/>
+      <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>

</xml_diff>

<commit_message>
Figures and edit - Intro (CC - Link with hibernation) - Figures - Edits in Chapter 1 - References
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49AE5E8-F6F5-EC41-9E38-F381EDB6968B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A64D1E3-4287-584C-B97C-0889DECDA4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29240" windowHeight="16860" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="188">
   <si>
     <t>Paper Title</t>
   </si>
@@ -689,12 +689,39 @@
   <si>
     <t>no evidence for general body mass reduction in response to climate change</t>
   </si>
+  <si>
+    <t>The handicap principle: a missing piece of darwin’s puzzle</t>
+  </si>
+  <si>
+    <t>Zahavi</t>
+  </si>
+  <si>
+    <t>Handicap principle</t>
+  </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>Julien???</t>
+  </si>
+  <si>
+    <t>Bigger is not always better: viability selection on body mass varies across life stages in a hibernating mammal</t>
+  </si>
+  <si>
+    <t>Ecology and Evolution</t>
+  </si>
+  <si>
+    <t>Jebb, Blumstein, Bize and Martin</t>
+  </si>
+  <si>
+    <t>The selective pressure is different according to IDs' age class because of different trade-offs (Young will have pressure for an average body mass to favor run speed when fleeing from a predator; Adults will have a pressure for a bigger body mass to insure survival over winter, as they rely on group vigilence while foraging in order to flee in time despite being slower because of their weight)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -835,6 +862,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -974,7 +1007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1069,6 +1102,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1407,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1960,8 +1996,8 @@
       <c r="I16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>13</v>
+      <c r="J16" s="35" t="s">
+        <v>182</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>12</v>
@@ -2061,7 +2097,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2103,7 +2139,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2137,7 +2173,7 @@
       </c>
       <c r="N21" s="18">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O21" s="19" t="s">
         <v>16</v>
@@ -2246,7 +2282,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2317,7 +2353,7 @@
       </c>
       <c r="N26" s="20">
         <f>COUNTIF(J:J, "no")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2339,8 +2375,8 @@
       <c r="I27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="5" t="s">
-        <v>13</v>
+      <c r="J27" s="35" t="s">
+        <v>182</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>12</v>
@@ -2817,31 +2853,69 @@
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="12"/>
+      <c r="A43" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1997</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>181</v>
+      </c>
       <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
+      <c r="I43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="8"/>
+      <c r="A44" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2021</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3340,6 +3414,7 @@
     <hyperlink ref="A21" r:id="rId3" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Blumstein_etal_2004_JM.pdf" xr:uid="{3A8C16DB-3B31-5A4F-8393-AE03B214C5D1}"/>
     <hyperlink ref="A22" r:id="rId4" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Blumstein_2009_JM.pdf" xr:uid="{25712E07-C75B-EE4C-A484-0AB3BB020C76}"/>
     <hyperlink ref="A23" r:id="rId5" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2020/03/Monclus_etal_2014_EvolEcol.pdf" xr:uid="{5C5293D3-C93C-8049-99C4-7FAB32E99F55}"/>
+    <hyperlink ref="A44" r:id="rId6" display="https://sites.lifesci.ucla.edu/eeb-rmbl-marmots/wp-content/uploads/sites/190/2021/03/Jebb_etal_2021_EcolEvol.pdf" xr:uid="{83CD597C-05ED-8C46-AAE5-F34497741365}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Intro edits (10.01.2025 (2))
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A64D1E3-4287-584C-B97C-0889DECDA4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE27C96-3024-DA4F-BB05-0F1CCB96116C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29240" windowHeight="16860" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="197">
   <si>
     <t>Paper Title</t>
   </si>
@@ -715,6 +715,33 @@
   </si>
   <si>
     <t>The selective pressure is different according to IDs' age class because of different trade-offs (Young will have pressure for an average body mass to favor run speed when fleeing from a predator; Adults will have a pressure for a bigger body mass to insure survival over winter, as they rely on group vigilence while foraging in order to flee in time despite being slower because of their weight)</t>
+  </si>
+  <si>
+    <t>Mammalian Hibernation: Cellular and Molecular Responses to Depressed Metabolism and Low Temperature</t>
+  </si>
+  <si>
+    <t>Physiological review</t>
+  </si>
+  <si>
+    <t>Carey, Andrews, Martin</t>
+  </si>
+  <si>
+    <t>Hibernation metabolism</t>
+  </si>
+  <si>
+    <t>An ecologist's guide to the animal model</t>
+  </si>
+  <si>
+    <t>Journal of Animal Ecology</t>
+  </si>
+  <si>
+    <t>Wilson, Réale, Clements, Morrissey, Postma, Walling, Kruuk &amp; Nussey</t>
+  </si>
+  <si>
+    <t>Global review on animal model (principle and utilisation)</t>
+  </si>
+  <si>
+    <t>animal model (ASREML, MCMCglmm)</t>
   </si>
 </sst>
 </file>
@@ -1443,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2097,7 +2124,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2139,7 +2166,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2173,7 +2200,7 @@
       </c>
       <c r="N21" s="18">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O21" s="19" t="s">
         <v>16</v>
@@ -2282,7 +2309,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2919,25 +2946,66 @@
       <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="A45" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2003</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="E45" s="2"/>
       <c r="F45" s="10"/>
-      <c r="G45" s="12"/>
+      <c r="G45" s="12" t="s">
+        <v>191</v>
+      </c>
       <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
+      <c r="I45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="F46" s="10"/>
-      <c r="J46" s="7"/>
+      <c r="A46" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>

</xml_diff>

<commit_message>
Introduction - Traits coevolution
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE27C96-3024-DA4F-BB05-0F1CCB96116C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52614073-6563-D64B-B57A-A868108A0C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29240" windowHeight="16860" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="206">
   <si>
     <t>Paper Title</t>
   </si>
@@ -743,12 +743,39 @@
   <si>
     <t>animal model (ASREML, MCMCglmm)</t>
   </si>
+  <si>
+    <t>VISUALIZING MULTIVARIATE SELECTION</t>
+  </si>
+  <si>
+    <t>Evolution</t>
+  </si>
+  <si>
+    <t>Phillips &amp; Arnolds</t>
+  </si>
+  <si>
+    <t>≈</t>
+  </si>
+  <si>
+    <t>Selection act on multiple traits rather than one</t>
+  </si>
+  <si>
+    <t>The adaptive landscape as a conceptual bridge between micro- and macroevolution</t>
+  </si>
+  <si>
+    <t>Springer Netherlands</t>
+  </si>
+  <si>
+    <t>Arnold et al.</t>
+  </si>
+  <si>
+    <t>Adaptive landscape (Review)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -895,6 +922,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1034,7 +1068,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1131,6 +1165,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1470,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:K46"/>
+    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2124,7 +2161,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2166,7 +2203,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2243,7 +2280,7 @@
       </c>
       <c r="N22" s="22">
         <f>COUNTIF(F:F, "no")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2309,7 +2346,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2959,7 +2996,9 @@
         <v>190</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="10"/>
+      <c r="F45" s="36" t="s">
+        <v>200</v>
+      </c>
       <c r="G45" s="12" t="s">
         <v>191</v>
       </c>
@@ -3008,28 +3047,64 @@
       </c>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="7"/>
+      <c r="A47" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1989</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>201</v>
+      </c>
       <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
+      <c r="I47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="A48" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2001</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
+      <c r="F48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>

</xml_diff>

<commit_message>
Bet-hedging, reference + figure chapter 2
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A77821-FC5A-0549-8B9D-D6A00CE2840A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAF1164-3AEC-5841-AE06-E4FCF0C5C7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29240" windowHeight="16860" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="227">
   <si>
     <t>Paper Title</t>
   </si>
@@ -805,6 +805,33 @@
   </si>
   <si>
     <t>Biro &amp; Stamps</t>
+  </si>
+  <si>
+    <t>Evolution and behavioural responses to human-induced rapid environmental change</t>
+  </si>
+  <si>
+    <t>Evolutionary application</t>
+  </si>
+  <si>
+    <t>Sih et al.</t>
+  </si>
+  <si>
+    <t>Evolution in response to human-induced changes</t>
+  </si>
+  <si>
+    <t>Ecological and evolutionary traps</t>
+  </si>
+  <si>
+    <t>Schlaepfer et al.</t>
+  </si>
+  <si>
+    <t>Evolutionary traps</t>
+  </si>
+  <si>
+    <t>Ecological novelty and the emergence of evolutionary traps</t>
+  </si>
+  <si>
+    <t>Robertson, Rehage &amp; Sih</t>
   </si>
 </sst>
 </file>
@@ -1532,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2186,7 +2213,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2228,7 +2255,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2305,7 +2332,7 @@
       </c>
       <c r="N22" s="22">
         <f>COUNTIF(F:F, "no")</f>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2371,7 +2398,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3256,41 +3283,96 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="2"/>
+      <c r="A53" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C53" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
+      <c r="I53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="6"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="A54" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="2">
+        <v>2002</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="E54" s="8"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="2"/>
+      <c r="F54" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="H54" s="8"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="7"/>
+      <c r="I54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="26"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="A55" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>226</v>
+      </c>
       <c r="E55" s="2"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="12"/>
+      <c r="F55" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
+      <c r="I55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11"/>

</xml_diff>

<commit_message>
Edits figure juvenile + material
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAF1164-3AEC-5841-AE06-E4FCF0C5C7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC8400A-2B8D-ED4E-A6A5-CB9AA2D81E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="900" windowWidth="29240" windowHeight="16860" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="29560" yWindow="660" windowWidth="18960" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="238">
   <si>
     <t>Paper Title</t>
   </si>
@@ -833,12 +833,45 @@
   <si>
     <t>Robertson, Rehage &amp; Sih</t>
   </si>
+  <si>
+    <t>The evolution of life histories</t>
+  </si>
+  <si>
+    <t>Stearns</t>
+  </si>
+  <si>
+    <t>LHT</t>
+  </si>
+  <si>
+    <t>Climate data from the Rocky Mountain Biological Laboratory (1975–2022)</t>
+  </si>
+  <si>
+    <t>Ecology</t>
+  </si>
+  <si>
+    <t>Prather, Underwood, Daldon, Barr, Inouye</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>RMBL weather data (1975-2022) citation</t>
+  </si>
+  <si>
+    <t>Climate in alpine habitat</t>
+  </si>
+  <si>
+    <t>HIGH ALTITUDE CLIMATES</t>
+  </si>
+  <si>
+    <t>Inouye, Wielgolaski</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -984,6 +1017,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1123,7 +1163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1220,6 +1260,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1559,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2213,7 +2256,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2255,7 +2298,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2289,7 +2332,7 @@
       </c>
       <c r="N21" s="18">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O21" s="19" t="s">
         <v>16</v>
@@ -2332,7 +2375,7 @@
       </c>
       <c r="N22" s="22">
         <f>COUNTIF(F:F, "no")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2398,7 +2441,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3375,42 +3418,100 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="11"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="12"/>
+      <c r="A56" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1992</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>229</v>
+      </c>
       <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
+      <c r="I56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J56" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="7"/>
+      <c r="A57" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E57" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>234</v>
+      </c>
       <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
+      <c r="I57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J57" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="6"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="2"/>
+      <c r="A58" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C58" s="2">
+        <v>2003</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F58" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>235</v>
+      </c>
       <c r="H58" s="8"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="7"/>
+      <c r="I58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>

</xml_diff>

<commit_message>
Adding study map and information about the data
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC8400A-2B8D-ED4E-A6A5-CB9AA2D81E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69275ED-8F97-E646-B491-F46A56B2F770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29560" yWindow="660" windowWidth="18960" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="246">
   <si>
     <t>Paper Title</t>
   </si>
@@ -865,6 +865,30 @@
   </si>
   <si>
     <t>Inouye, Wielgolaski</t>
+  </si>
+  <si>
+    <t>GIS Mapping Software, Location Intelligence &amp; Spatial Analytics</t>
+  </si>
+  <si>
+    <t>ESRI</t>
+  </si>
+  <si>
+    <t>ESRI base map citation</t>
+  </si>
+  <si>
+    <t>GIS</t>
+  </si>
+  <si>
+    <t>QGIS Geographic Information System [Computer software]</t>
+  </si>
+  <si>
+    <t>QGIS</t>
+  </si>
+  <si>
+    <t>QGIS developpment team</t>
+  </si>
+  <si>
+    <t>QGIS software citation</t>
   </si>
 </sst>
 </file>
@@ -1602,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2256,7 +2280,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2298,7 +2322,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2339,7 +2363,7 @@
       </c>
       <c r="P21" s="20">
         <f>COUNTIF(E:E, "Software/Package")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2441,7 +2465,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3514,30 +3538,74 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
+      <c r="A59" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C59" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="11"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
+      <c r="A60" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C60" s="2">
+        <v>2024</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="24"/>

</xml_diff>

<commit_message>
Proof-reading till traits coevolution
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69275ED-8F97-E646-B491-F46A56B2F770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E449BCB-8AAC-BA42-8F62-575A4B3478FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29560" yWindow="660" windowWidth="18960" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -1626,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2027,7 +2027,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
updates chapters 1 and figure 2
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43304392-1FF0-AF4C-95DD-3FA8DEEC50F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73A5F11-6D98-DF48-AFE7-CCB6559CA712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29560" yWindow="660" windowWidth="18960" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="270">
   <si>
     <t>Paper Title</t>
   </si>
@@ -946,6 +946,21 @@
   </si>
   <si>
     <t>Abstract, Method</t>
+  </si>
+  <si>
+    <t>Analysis of Ecological Data: Exploratory and Euclidean Methods in Environmental Sciences (ade4)</t>
+  </si>
+  <si>
+    <t>CRAN</t>
+  </si>
+  <si>
+    <t>Dray, Dufour, Thioulouse &amp; Siberchicot</t>
+  </si>
+  <si>
+    <t>ade4 package description</t>
+  </si>
+  <si>
+    <t>Multivariate statistics</t>
   </si>
 </sst>
 </file>
@@ -1691,7 +1706,7 @@
   <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:K65"/>
+      <selection activeCell="A66" sqref="A66:K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2344,7 +2359,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2386,7 +2401,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2427,7 +2442,7 @@
       </c>
       <c r="P21" s="20">
         <f>COUNTIF(E:E, "Software/Package")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2529,7 +2544,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3832,17 +3847,39 @@
       </c>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
+      <c r="A66" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C66" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>

</xml_diff>

<commit_message>
adds - chapter 2
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1358CC8-D6DE-7B46-8AF0-47B4BED31CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3D46F6-631A-AC4E-A527-4DDA919F76CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="500" windowWidth="21140" windowHeight="21100" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="29400" yWindow="500" windowWidth="21140" windowHeight="19880" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="273">
   <si>
     <t>Paper Title</t>
   </si>
@@ -961,6 +961,15 @@
   </si>
   <si>
     <t>Multivariate statistics</t>
+  </si>
+  <si>
+    <t>Stan: A Probabilistic Programming Language</t>
+  </si>
+  <si>
+    <t>Carpenter et al.</t>
+  </si>
+  <si>
+    <t>Stan software</t>
   </si>
 </sst>
 </file>
@@ -1705,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:K85"/>
+    <sheetView tabSelected="1" topLeftCell="H38" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2359,7 +2368,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2401,7 +2410,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2442,7 +2451,7 @@
       </c>
       <c r="P21" s="20">
         <f>COUNTIF(E:E, "Software/Package")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2544,7 +2553,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3882,17 +3891,37 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="2"/>
+      <c r="A67" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>272</v>
+      </c>
       <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
+      <c r="I67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>

</xml_diff>

<commit_message>
plasticity vs evolution - rewrite
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3D46F6-631A-AC4E-A527-4DDA919F76CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077AB18E-F1F9-814C-A066-8601F75E86EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="500" windowWidth="21140" windowHeight="19880" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="277">
   <si>
     <t>Paper Title</t>
   </si>
@@ -970,6 +970,18 @@
   </si>
   <si>
     <t>Stan software</t>
+  </si>
+  <si>
+    <t>Phenotypic plasticity: beyond nature and nurture</t>
+  </si>
+  <si>
+    <t>JHU Press</t>
+  </si>
+  <si>
+    <t>Pigliucci</t>
+  </si>
+  <si>
+    <t>Phenotypic plasticity</t>
   </si>
 </sst>
 </file>
@@ -1714,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H38" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67"/>
+    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2368,7 +2380,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2553,7 +2565,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2624,7 +2636,7 @@
       </c>
       <c r="N26" s="20">
         <f>COUNTIF(J:J, "no")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3924,17 +3936,37 @@
       </c>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="3"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="2"/>
+      <c r="A68" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C68" s="2">
+        <v>2001</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
+      <c r="I68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>

</xml_diff>

<commit_message>
added 2 citations (Grabbher, 2010; TMB)
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077AB18E-F1F9-814C-A066-8601F75E86EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F6A726-769F-934A-9B67-C201FD834DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="500" windowWidth="21140" windowHeight="19880" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="33880" yWindow="3200" windowWidth="29400" windowHeight="17220" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="284">
   <si>
     <t>Paper Title</t>
   </si>
@@ -982,6 +982,27 @@
   </si>
   <si>
     <t>Phenotypic plasticity</t>
+  </si>
+  <si>
+    <t>Climate Change Impacts in Alpine Environments</t>
+  </si>
+  <si>
+    <t>Geography compass</t>
+  </si>
+  <si>
+    <t>Grabherr, Gottfried &amp; Pauli</t>
+  </si>
+  <si>
+    <t>Climate change in Apline environment</t>
+  </si>
+  <si>
+    <t>TMB: Automatic Differentiation and Laplace Approximation</t>
+  </si>
+  <si>
+    <t>Kristensen &amp; al.</t>
+  </si>
+  <si>
+    <t>TMB package</t>
   </si>
 </sst>
 </file>
@@ -1726,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2380,7 +2401,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2422,7 +2443,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2463,7 +2484,7 @@
       </c>
       <c r="P21" s="20">
         <f>COUNTIF(E:E, "Software/Package")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2565,7 +2586,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3969,30 +3990,68 @@
       </c>
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="A69" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C69" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>279</v>
+      </c>
       <c r="E69" s="13"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="2"/>
+      <c r="F69" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>280</v>
+      </c>
       <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
+      <c r="I69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="11"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="12"/>
+      <c r="A70" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="2">
+        <v>2016</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>283</v>
+      </c>
       <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
+      <c r="I70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>

</xml_diff>

<commit_message>
correction climate change + link with body mass as a LHT
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F6A726-769F-934A-9B67-C201FD834DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665F0C79-881D-004F-856A-636422C2F53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33880" yWindow="3200" windowWidth="29400" windowHeight="17220" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="160" yWindow="900" windowWidth="29100" windowHeight="16920" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="299">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1003,6 +1003,51 @@
   </si>
   <si>
     <t>TMB package</t>
+  </si>
+  <si>
+    <t>Enhanced temperature variability in high-altitude climate change</t>
+  </si>
+  <si>
+    <t>Theoritical and Applied Climatology</t>
+  </si>
+  <si>
+    <t>Ohmura</t>
+  </si>
+  <si>
+    <t>Temperature variability in high altitude</t>
+  </si>
+  <si>
+    <t>Climates of the Rocky Mountains: Historical and Future Patterns</t>
+  </si>
+  <si>
+    <t>Ø</t>
+  </si>
+  <si>
+    <t>Kittel, Thornton, Royle, Chase</t>
+  </si>
+  <si>
+    <t>Droughts</t>
+  </si>
+  <si>
+    <t>Elevation Dependency of the Surface Climate Change Signal: A Model Study</t>
+  </si>
+  <si>
+    <t>Journal of Climate</t>
+  </si>
+  <si>
+    <t>Giorgi, Hurrell, Marinucci, Beniston</t>
+  </si>
+  <si>
+    <t>"more pronounced warming at high elevation"</t>
+  </si>
+  <si>
+    <t>The Costs of Reproduction and Their Consequences</t>
+  </si>
+  <si>
+    <t>The american naturalist</t>
+  </si>
+  <si>
+    <t>Bell</t>
   </si>
 </sst>
 </file>
@@ -1747,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" topLeftCell="E62" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2401,7 +2446,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2443,7 +2488,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2520,7 +2565,7 @@
       </c>
       <c r="N22" s="22">
         <f>COUNTIF(F:F, "no")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2586,7 +2631,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4054,56 +4099,130 @@
       </c>
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="3"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="A71" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C71" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="E71" s="13"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="2"/>
+      <c r="F71" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
+      <c r="I71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="2"/>
+      <c r="A72" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C72" s="2">
+        <v>2002</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F72" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>291</v>
+      </c>
       <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="K72" s="2"/>
+      <c r="I72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
+      <c r="A73" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C73" s="2">
+        <v>1997</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>294</v>
+      </c>
       <c r="E73" s="13"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="2"/>
+      <c r="F73" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
+      <c r="I73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="A74" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1980</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="E74" s="13"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="2"/>
+      <c r="F74" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
+      <c r="I74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>

</xml_diff>

<commit_message>
correction - BM a LHT
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665F0C79-881D-004F-856A-636422C2F53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB707A7C-2444-0B4F-A554-51000059C510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29100" windowHeight="16920" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="304">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1048,6 +1048,21 @@
   </si>
   <si>
     <t>Bell</t>
+  </si>
+  <si>
+    <t>How do mammals buffer environmental seasonality? The role of brain size, body fat and allomaternal care in dealing with energy shortage</t>
+  </si>
+  <si>
+    <t>University of Zurich</t>
+  </si>
+  <si>
+    <t>Heldstab</t>
+  </si>
+  <si>
+    <t>PhD Thesis</t>
+  </si>
+  <si>
+    <t>§ in the intro: "How do mammals cope with seasonal food scarcity?" &gt; "Physiological buffering" &gt; "body fat storage"</t>
   </si>
 </sst>
 </file>
@@ -1792,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E62" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" topLeftCell="E57" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2446,7 +2461,7 @@
       </c>
       <c r="N19" s="15">
         <f>N20+N26</f>
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2488,7 +2503,7 @@
       </c>
       <c r="N20" s="15">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2631,7 +2646,7 @@
       </c>
       <c r="N24" s="20">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4225,16 +4240,37 @@
       </c>
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="2"/>
+      <c r="A75" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C75" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="F75" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>303</v>
+      </c>
       <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
+      <c r="I75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>

</xml_diff>

<commit_message>
correction - introduction end
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB707A7C-2444-0B4F-A554-51000059C510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1D6871-EFD6-694C-BFB0-7E0282980CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29100" windowHeight="16920" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="339">
   <si>
     <t>Paper Title</t>
   </si>
@@ -352,32 +352,6 @@
     <t>The biology hidden inside residual within-individual phenotypic variation</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Recent increase in body size of the American merten </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Martes americana </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in Alaska</t>
-    </r>
-  </si>
-  <si>
     <t>Biological Journal of the Linnean Society</t>
   </si>
   <si>
@@ -1064,12 +1038,141 @@
   <si>
     <t>§ in the intro: "How do mammals cope with seasonal food scarcity?" &gt; "Physiological buffering" &gt; "body fat storage"</t>
   </si>
+  <si>
+    <t>Bird migration</t>
+  </si>
+  <si>
+    <t>Alerstam, Christie</t>
+  </si>
+  <si>
+    <t>bird migration</t>
+  </si>
+  <si>
+    <t>Population‐specific adjustment of the annual cycle in a super‐swift trans‐Saharan migrant</t>
+  </si>
+  <si>
+    <t>Journal of Avian Biology</t>
+  </si>
+  <si>
+    <t>Meier et al.</t>
+  </si>
+  <si>
+    <t>Migration in Alpine swifts</t>
+  </si>
+  <si>
+    <t>Understanding Evolutionary Impacts of Seasonality: An Introduction to the Symposium</t>
+  </si>
+  <si>
+    <t>Integrative and comparative biology</t>
+  </si>
+  <si>
+    <t>Williams et al.</t>
+  </si>
+  <si>
+    <t>Notion of seasonality</t>
+  </si>
+  <si>
+    <t>Over-winter activity and body temperature patterns in northern beavers</t>
+  </si>
+  <si>
+    <t>Canadian Journal of Zoology</t>
+  </si>
+  <si>
+    <t>Smith et al.</t>
+  </si>
+  <si>
+    <t>Beavers' ecology in winter</t>
+  </si>
+  <si>
+    <t>Castor canadensis</t>
+  </si>
+  <si>
+    <t>Mammalian species</t>
+  </si>
+  <si>
+    <t>Jenkins, Busher</t>
+  </si>
+  <si>
+    <t>Survival of the fattest: How body fat and migration influence survival in highly seasonal environments</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Recent increase in body size of the American merten </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Martes americana </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in Alaska</t>
+    </r>
+  </si>
+  <si>
+    <t>Functional Ecology</t>
+  </si>
+  <si>
+    <t>Denryter et al.</t>
+  </si>
+  <si>
+    <t>Body fat &lt;=&gt; Buffer</t>
+  </si>
+  <si>
+    <t>Linking population performance to nutritional condition in an alpine ungulate</t>
+  </si>
+  <si>
+    <t>Journal of Mammalogy</t>
+  </si>
+  <si>
+    <t>Stephenson et al.</t>
+  </si>
+  <si>
+    <t>Body fat in bighorn sheep</t>
+  </si>
+  <si>
+    <t>Body mass dependent use of hibernation: why not prolong the active season, if they can?</t>
+  </si>
+  <si>
+    <t>Bieber et al.</t>
+  </si>
+  <si>
+    <t>Chimpunk are food-storing hibernators</t>
+  </si>
+  <si>
+    <t>Evolution of phenotypic plasticity: where are we going now?</t>
+  </si>
+  <si>
+    <t>evolution of PP</t>
+  </si>
+  <si>
+    <t>The analysis of adaptation in a plant-breeding programme</t>
+  </si>
+  <si>
+    <t>Australian Journal of Agricultural Research</t>
+  </si>
+  <si>
+    <t>Finlay, Wilkison</t>
+  </si>
+  <si>
+    <t>Ramakers et al. 2023's original method</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1140,13 +1243,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1195,14 +1291,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="6"/>
       <name val="Calibri"/>
@@ -1228,6 +1316,26 @@
       <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1398,13 +1506,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1437,19 +1542,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1458,16 +1560,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1807,13 +1919,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E57" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75"/>
+    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59" customWidth="1"/>
+    <col min="1" max="1" width="59" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="6.5" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
@@ -1829,7 +1941,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1865,7 +1977,7 @@
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1883,7 +1995,7 @@
       <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
         <v>12</v>
@@ -1937,7 +2049,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="34" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1955,7 +2067,7 @@
       <c r="F4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
         <v>12</v>
@@ -1963,12 +2075,12 @@
       <c r="J4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="34" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1986,7 +2098,7 @@
       <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>80</v>
       </c>
       <c r="H5" s="2"/>
@@ -2001,7 +2113,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="34" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2019,7 +2131,7 @@
       <c r="F6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>83</v>
       </c>
       <c r="H6" s="2"/>
@@ -2035,16 +2147,16 @@
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="C7" s="2">
         <v>2014</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>79</v>
@@ -2053,7 +2165,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
@@ -2067,7 +2179,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2083,7 +2195,7 @@
       <c r="F8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>35</v>
       </c>
       <c r="H8" s="2"/>
@@ -2102,7 +2214,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2114,7 +2226,7 @@
       <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -2135,7 +2247,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2171,7 +2283,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2183,7 +2295,7 @@
       <c r="D11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -2201,7 +2313,7 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="34" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2219,7 +2331,7 @@
       <c r="F12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="2"/>
@@ -2235,7 +2347,7 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="34" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2269,7 +2381,7 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="34" t="s">
         <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2303,7 +2415,7 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="34" t="s">
         <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2318,10 +2430,10 @@
       <c r="E15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="12" t="s">
+      <c r="F15" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>67</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -2338,7 +2450,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="34" t="s">
         <v>69</v>
       </c>
       <c r="B16" s="2"/>
@@ -2348,7 +2460,7 @@
       <c r="D16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="27" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -2360,8 +2472,8 @@
       <c r="I16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="33" t="s">
-        <v>182</v>
+      <c r="J16" s="29" t="s">
+        <v>181</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>12</v>
@@ -2384,7 +2496,7 @@
       <c r="F17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="11" t="s">
         <v>75</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -2398,53 +2510,53 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C18" s="2">
         <v>2008</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F18" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="I18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C19" s="2">
         <v>2015</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>12</v>
@@ -2452,24 +2564,24 @@
       <c r="J19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="36" t="s">
         <v>13</v>
       </c>
       <c r="L19" s="2"/>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="C20" s="8">
         <v>1965</v>
@@ -2478,46 +2590,46 @@
         <v>24</v>
       </c>
       <c r="E20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="I20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="14">
+        <f>COUNTIF(J:J, "yes")</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="N20" s="15">
-        <f>COUNTIF(J:J, "yes")</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
+      <c r="B21" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C21" s="2">
         <v>2004</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>13</v>
@@ -2532,33 +2644,33 @@
       <c r="K21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M21" s="17" t="s">
+      <c r="M21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="N21" s="18">
+      <c r="N21" s="17">
         <f>COUNTIF(F:F, "yes")</f>
         <v>20</v>
       </c>
-      <c r="O21" s="19" t="s">
+      <c r="O21" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="P21" s="20">
+      <c r="P21" s="19">
         <f>COUNTIF(E:E, "Software/Package")</f>
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="s">
-        <v>100</v>
+      <c r="A22" s="33" t="s">
+        <v>99</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="2">
         <v>2009</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="10" t="s">
@@ -2575,26 +2687,26 @@
       <c r="K22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M22" s="21" t="s">
+      <c r="M22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N22" s="22">
+      <c r="N22" s="21">
         <f>COUNTIF(F:F, "no")</f>
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C23" s="2">
         <v>2014</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>13</v>
@@ -2614,44 +2726,44 @@
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="C24" s="2">
         <v>2023</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="I24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="N24" s="19">
+        <f>COUNTIF(K:K, "yes")</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="34" t="s">
         <v>108</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M24" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="N24" s="20">
-        <f>COUNTIF(K:K, "yes")</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
@@ -2660,7 +2772,7 @@
         <v>1859</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>25</v>
@@ -2668,8 +2780,8 @@
       <c r="F25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="12" t="s">
-        <v>111</v>
+      <c r="G25" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2" t="s">
@@ -2685,7 +2797,7 @@
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>41</v>
@@ -2694,14 +2806,14 @@
         <v>1998</v>
       </c>
       <c r="D26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="I26" s="2" t="s">
         <v>12</v>
       </c>
@@ -2712,26 +2824,26 @@
         <v>12</v>
       </c>
       <c r="L26" s="8"/>
-      <c r="M26" s="23" t="s">
+      <c r="M26" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="19">
         <f>COUNTIF(J:J, "no")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C27" s="2">
         <v>1998</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>11</v>
@@ -2739,8 +2851,8 @@
       <c r="I27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="33" t="s">
-        <v>182</v>
+      <c r="J27" s="29" t="s">
+        <v>181</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>12</v>
@@ -2749,81 +2861,81 @@
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="C28" s="2">
         <v>1979</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>89</v>
+      <c r="B29" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="C29" s="2">
         <v>2012</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>129</v>
-      </c>
       <c r="B30" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C30" s="2">
         <v>2002</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>132</v>
+      <c r="G30" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2" t="s">
@@ -2838,22 +2950,22 @@
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="C31" s="2">
         <v>2005</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="12" t="s">
-        <v>132</v>
+      <c r="G31" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="2" t="s">
@@ -2868,28 +2980,28 @@
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="C32" s="2">
         <v>2024</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="F32" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F32" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>12</v>
@@ -2903,60 +3015,60 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="C33" s="2">
         <v>2024</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>139</v>
+        <v>143</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
+      <c r="B34" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="C34" s="2">
         <v>2010</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>139</v>
+        <v>147</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="12" t="s">
-        <v>149</v>
+      <c r="G34" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
@@ -2970,26 +3082,26 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>152</v>
+      <c r="A35" s="34" t="s">
+        <v>151</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C35" s="2">
         <v>2021</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>139</v>
+        <v>149</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="12" t="s">
-        <v>151</v>
+      <c r="G35" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
@@ -3004,26 +3116,26 @@
       <c r="L35" s="8"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="C36" s="2">
         <v>2016</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>139</v>
+        <v>154</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="12" t="s">
-        <v>156</v>
+      <c r="G36" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="s">
@@ -3038,52 +3150,52 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="C37" s="2">
         <v>2022</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G37" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
+      <c r="B38" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="C38" s="2">
         <v>2019</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>12</v>
@@ -3097,52 +3209,52 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="C39" s="2">
         <v>2013</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="12" t="s">
+      <c r="G39" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B40" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="C40" s="2">
         <v>1990</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="s">
@@ -3156,53 +3268,53 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>172</v>
+      <c r="A41" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="2">
         <v>2007</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>176</v>
-      </c>
       <c r="B42" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42" s="2">
         <v>2019</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
@@ -3217,8 +3329,8 @@
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>179</v>
+      <c r="A43" s="34" t="s">
+        <v>178</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>31</v>
@@ -3227,7 +3339,7 @@
         <v>1997</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>25</v>
@@ -3235,40 +3347,40 @@
       <c r="F43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G43" s="12" t="s">
-        <v>181</v>
+      <c r="G43" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J43" s="33" t="s">
+      <c r="J43" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="K43" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
+      <c r="B44" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="C44" s="2">
         <v>2021</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>187</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="s">
@@ -3283,24 +3395,24 @@
       <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="C45" s="2">
         <v>2003</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G45" s="11" t="s">
         <v>190</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>191</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2" t="s">
@@ -3314,27 +3426,27 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="C46" s="2">
         <v>2010</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="12" t="s">
+      <c r="H46" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>12</v>
@@ -3348,22 +3460,22 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>198</v>
       </c>
       <c r="C47" s="2">
         <v>1989</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="2" t="s">
@@ -3378,23 +3490,23 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="C48" s="2">
         <v>2001</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>12</v>
@@ -3408,23 +3520,23 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="C49" s="2">
         <v>2010</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="2" t="s">
@@ -3439,23 +3551,23 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>210</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>211</v>
       </c>
       <c r="C50" s="2">
         <v>2007</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="2" t="s">
@@ -3471,7 +3583,7 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>64</v>
@@ -3480,14 +3592,14 @@
         <v>2007</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="2" t="s">
@@ -3502,7 +3614,7 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>41</v>
@@ -3511,14 +3623,14 @@
         <v>2008</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>12</v>
@@ -3532,22 +3644,22 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="C53" s="2">
         <v>2011</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2" t="s">
@@ -3562,7 +3674,7 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>41</v>
@@ -3571,14 +3683,14 @@
         <v>2002</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="2" t="s">
@@ -3592,8 +3704,8 @@
       </c>
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="26" t="s">
-        <v>225</v>
+      <c r="A55" s="33" t="s">
+        <v>224</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>41</v>
@@ -3602,14 +3714,14 @@
         <v>2013</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2" t="s">
@@ -3623,8 +3735,8 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
-        <v>227</v>
+      <c r="A56" s="34" t="s">
+        <v>226</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>31</v>
@@ -3633,7 +3745,7 @@
         <v>1992</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>25</v>
@@ -3641,15 +3753,15 @@
       <c r="F56" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G56" s="12" t="s">
-        <v>229</v>
+      <c r="G56" s="11" t="s">
+        <v>228</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J56" s="33" t="s">
-        <v>183</v>
+      <c r="J56" s="29" t="s">
+        <v>182</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>12</v>
@@ -3657,32 +3769,32 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="C57" s="2">
         <v>2023</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E57" s="31" t="s">
         <v>232</v>
-      </c>
-      <c r="E57" s="35" t="s">
-        <v>233</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J57" s="33" t="s">
-        <v>183</v>
+      <c r="J57" s="29" t="s">
+        <v>182</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>12</v>
@@ -3690,25 +3802,25 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C58" s="2">
         <v>2003</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F58" s="34" t="s">
-        <v>200</v>
+      <c r="F58" s="30" t="s">
+        <v>199</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="2" t="s">
@@ -3723,28 +3835,28 @@
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="C59" s="2">
         <v>2024</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>139</v>
+        <v>237</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G59" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>12</v>
@@ -3758,60 +3870,60 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="C60" s="2">
         <v>2024</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>139</v>
+        <v>242</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="24" t="s">
+      <c r="B61" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="C61" s="2">
         <v>2006</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>139</v>
+        <v>246</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2" t="s">
@@ -3825,24 +3937,24 @@
       </c>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="11" t="s">
-        <v>250</v>
+      <c r="A62" s="34" t="s">
+        <v>249</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C62" s="2">
         <v>2010</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G62" s="11" t="s">
         <v>251</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="G62" s="12" t="s">
-        <v>252</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2" t="s">
@@ -3856,24 +3968,24 @@
       </c>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="C63" s="2">
         <v>1966</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G63" s="12" t="s">
-        <v>256</v>
+      <c r="G63" s="11" t="s">
+        <v>255</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2" t="s">
@@ -3887,24 +3999,24 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="C64" s="2">
         <v>2010</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="11" t="s">
         <v>259</v>
-      </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="12" t="s">
-        <v>260</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2" t="s">
@@ -3918,24 +4030,24 @@
       </c>
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="C65" s="2">
         <v>2012</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="36" t="s">
-        <v>264</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>260</v>
+      <c r="G65" s="11" t="s">
+        <v>259</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2" t="s">
@@ -3950,28 +4062,28 @@
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="C66" s="2">
         <v>2023</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E66" s="13" t="s">
-        <v>139</v>
+        <v>266</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G66" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H66" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>12</v>
@@ -3985,25 +4097,25 @@
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C67" s="2">
         <v>2017</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>139</v>
+        <v>270</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2" t="s">
@@ -4018,31 +4130,31 @@
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="C68" s="2">
         <v>2001</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E68" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="E68" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J68" s="5" t="s">
         <v>13</v>
       </c>
       <c r="K68" s="2" t="s">
@@ -4051,23 +4163,23 @@
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="C69" s="2">
         <v>2010</v>
       </c>
       <c r="D69" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E69" s="12"/>
+      <c r="F69" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="E69" s="13"/>
-      <c r="F69" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2" t="s">
@@ -4081,26 +4193,26 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="11" t="s">
-        <v>281</v>
+      <c r="A70" s="34" t="s">
+        <v>280</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C70" s="2">
         <v>2016</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>139</v>
+        <v>281</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G70" s="12" t="s">
-        <v>283</v>
+      <c r="G70" s="11" t="s">
+        <v>282</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2" t="s">
@@ -4115,23 +4227,23 @@
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="C71" s="2">
         <v>2012</v>
       </c>
       <c r="D71" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E71" s="12"/>
+      <c r="F71" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="E71" s="13"/>
-      <c r="F71" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2" t="s">
@@ -4146,25 +4258,25 @@
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="C72" s="2">
         <v>2002</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F72" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F72" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>291</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2" t="s">
@@ -4179,23 +4291,23 @@
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="C73" s="2">
         <v>1997</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E73" s="12"/>
+      <c r="F73" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="E73" s="13"/>
-      <c r="F73" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2" t="s">
@@ -4210,23 +4322,23 @@
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="C74" s="2">
         <v>1980</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E74" s="13"/>
+        <v>297</v>
+      </c>
+      <c r="E74" s="12"/>
       <c r="F74" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2" t="s">
@@ -4241,25 +4353,25 @@
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="C75" s="2">
         <v>2017</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E75" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="E75" s="13" t="s">
+      <c r="F75" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G75" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="F75" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2" t="s">
@@ -4273,105 +4385,297 @@
       </c>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="3"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
+      <c r="A76" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="2">
+        <v>2004</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="3"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
+      <c r="A77" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C77" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="3"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="F78" s="10"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
+      <c r="A78" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C78" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="28"/>
-      <c r="F79" s="10"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
+      <c r="A79" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C79" s="2">
+        <v>1991</v>
+      </c>
+      <c r="D79" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="F79" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="29"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
+      <c r="A80" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C80" s="2">
+        <v>1979</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F80" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="29"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="F81" s="10"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
+      <c r="A81" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C81" s="2">
+        <v>2022</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F81" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="24"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="F82" s="10"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
+      <c r="A82" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C82" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F82" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="24"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="F83" s="10"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
-      <c r="K83" s="2"/>
+      <c r="A83" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C83" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F83" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="29"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="F84" s="10"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" s="29"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="F85" s="10"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
+      <c r="A84" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84" s="2">
+        <v>2005</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F84" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A85" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1963</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
remake - chapter 1
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57201080-BA10-1843-93F2-DE0A39FD5AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4522CF-6CDB-004A-A33F-AD0378C4715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="900" windowWidth="29100" windowHeight="16920" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="29460" yWindow="500" windowWidth="29100" windowHeight="16920" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="386">
   <si>
     <t>Paper Title</t>
   </si>
@@ -994,9 +994,6 @@
     <t>Climates of the Rocky Mountains: Historical and Future Patterns</t>
   </si>
   <si>
-    <t>Ø</t>
-  </si>
-  <si>
     <t>Kittel, Thornton, Royle, Chase</t>
   </si>
   <si>
@@ -1244,6 +1241,72 @@
   </si>
   <si>
     <t>Fest-bianchet, Gaillard, Jorgenson</t>
+  </si>
+  <si>
+    <t>The role of body mass in thermoregulation</t>
+  </si>
+  <si>
+    <t>American Journal of Physical Anthropology</t>
+  </si>
+  <si>
+    <t>Riesenfield</t>
+  </si>
+  <si>
+    <t>large body mass =&gt; better with cold ; small body mass =&gt; better with heat</t>
+  </si>
+  <si>
+    <t>Physiology of thermoregulation</t>
+  </si>
+  <si>
+    <t>Best Practice &amp; Research Clinical Anaesthesiology</t>
+  </si>
+  <si>
+    <t>Kurz</t>
+  </si>
+  <si>
+    <t>Plots showing significant effect of body mass and fat on core T°</t>
+  </si>
+  <si>
+    <t>Effects of food abundance and predictability on body condition and health parameters: experimental tests with the Hooded Crow</t>
+  </si>
+  <si>
+    <t>Ibis</t>
+  </si>
+  <si>
+    <t>Acquarone et al.</t>
+  </si>
+  <si>
+    <t>link between body mass and food abundance</t>
+  </si>
+  <si>
+    <t>On the uses of data on lifetime reproductive success</t>
+  </si>
+  <si>
+    <t>Reproductive success. Studies of individual variation in contrasting breeding systems</t>
+  </si>
+  <si>
+    <t>Grafen</t>
+  </si>
+  <si>
+    <t>Invisible fraction definition (apparently)</t>
+  </si>
+  <si>
+    <t>The missing fraction problem as an episodes of selection problem</t>
+  </si>
+  <si>
+    <t>Evolution (Manuscript)</t>
+  </si>
+  <si>
+    <t>Mittell &amp; Morrisey</t>
+  </si>
+  <si>
+    <t>Missing fraction explanation</t>
+  </si>
+  <si>
+    <t>Missing fraction idea</t>
+  </si>
+  <si>
+    <t>Estimating evolutionary parameters when viability selection is operating</t>
   </si>
 </sst>
 </file>
@@ -1554,7 +1617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1660,14 +1723,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2005,10 +2067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E62" workbookViewId="0">
-      <selection activeCell="K92" sqref="K92"/>
+    <sheetView tabSelected="1" topLeftCell="E69" workbookViewId="0">
+      <selection activeCell="K98" sqref="K98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2016,7 +2078,7 @@
     <col min="1" max="1" width="59" style="3" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="6.5" customWidth="1"/>
-    <col min="4" max="4" width="30.5" style="39" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="139.33203125" customWidth="1"/>
@@ -2032,13 +2094,13 @@
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -2068,7 +2130,7 @@
       <c r="A2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="2">
@@ -2111,7 +2173,7 @@
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="2">
@@ -2140,7 +2202,7 @@
       <c r="A4" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="2">
@@ -2171,7 +2233,7 @@
       <c r="A5" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="2">
@@ -2204,7 +2266,7 @@
       <c r="A6" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="2">
@@ -2237,7 +2299,7 @@
       <c r="A7" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="25" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="2">
@@ -2270,7 +2332,7 @@
       <c r="A8" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="28" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="2">
@@ -2305,7 +2367,7 @@
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="2">
@@ -2338,7 +2400,7 @@
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="2">
@@ -2374,7 +2436,7 @@
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="28" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="2">
@@ -2404,7 +2466,7 @@
       <c r="A12" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2">
@@ -2438,7 +2500,7 @@
       <c r="A13" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="28" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="2">
@@ -2472,7 +2534,7 @@
       <c r="A14" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="28" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="2">
@@ -2506,7 +2568,7 @@
       <c r="A15" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="28" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="2">
@@ -2541,7 +2603,7 @@
       <c r="A16" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="2">
         <v>1992</v>
       </c>
@@ -2572,13 +2634,13 @@
       <c r="A17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="25" t="s">
         <v>73</v>
       </c>
       <c r="C17" s="2">
         <v>2011</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" t="s">
         <v>74</v>
       </c>
       <c r="F17" s="9" t="s">
@@ -2599,9 +2661,9 @@
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="B18" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>85</v>
       </c>
       <c r="C18" s="2">
@@ -2631,7 +2693,7 @@
       <c r="A19" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="28" t="s">
         <v>88</v>
       </c>
       <c r="C19" s="2">
@@ -2661,20 +2723,20 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="38" t="s">
         <v>92</v>
       </c>
       <c r="C20" s="8">
         <v>1965</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="38" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -2703,14 +2765,14 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="28" t="s">
         <v>97</v>
       </c>
       <c r="C21" s="2">
@@ -2751,7 +2813,7 @@
       <c r="A22" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="28" t="s">
         <v>97</v>
       </c>
       <c r="C22" s="2">
@@ -2780,14 +2842,14 @@
       </c>
       <c r="N22" s="21">
         <f>COUNTIF(F:F, "no")</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="28" t="s">
         <v>102</v>
       </c>
       <c r="C23" s="2">
@@ -2817,7 +2879,7 @@
       <c r="A24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="28" t="s">
         <v>105</v>
       </c>
       <c r="C24" s="2">
@@ -2846,14 +2908,14 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="2">
@@ -2887,13 +2949,13 @@
       <c r="A26" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="2">
         <v>1998</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="D26" t="s">
         <v>112</v>
       </c>
       <c r="F26" s="9" t="s">
@@ -2924,7 +2986,7 @@
       <c r="A27" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="28" t="s">
         <v>119</v>
       </c>
       <c r="C27" s="2">
@@ -2951,7 +3013,7 @@
       <c r="A28" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="28" t="s">
         <v>122</v>
       </c>
       <c r="C28" s="2">
@@ -3009,7 +3071,7 @@
       <c r="A30" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="28" t="s">
         <v>130</v>
       </c>
       <c r="C30" s="2">
@@ -3040,7 +3102,7 @@
       <c r="A31" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="25" t="s">
         <v>133</v>
       </c>
       <c r="C31" s="2">
@@ -3070,7 +3132,7 @@
       <c r="A32" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="28" t="s">
         <v>136</v>
       </c>
       <c r="C32" s="2">
@@ -3105,7 +3167,7 @@
       <c r="A33" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="28" t="s">
         <v>142</v>
       </c>
       <c r="C33" s="2">
@@ -3140,7 +3202,7 @@
       <c r="A34" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="28" t="s">
         <v>146</v>
       </c>
       <c r="C34" s="2">
@@ -3173,7 +3235,7 @@
       <c r="A35" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="28" t="s">
         <v>146</v>
       </c>
       <c r="C35" s="2">
@@ -3207,7 +3269,7 @@
       <c r="A36" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="28" t="s">
         <v>153</v>
       </c>
       <c r="C36" s="2">
@@ -3240,7 +3302,7 @@
       <c r="A37" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="25" t="s">
         <v>157</v>
       </c>
       <c r="C37" s="2">
@@ -3270,7 +3332,7 @@
       <c r="A38" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="28" t="s">
         <v>161</v>
       </c>
       <c r="C38" s="2">
@@ -3299,7 +3361,7 @@
       <c r="A39" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="25" t="s">
         <v>165</v>
       </c>
       <c r="C39" s="2">
@@ -3329,7 +3391,7 @@
       <c r="A40" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="28" t="s">
         <v>169</v>
       </c>
       <c r="C40" s="2">
@@ -3359,7 +3421,7 @@
       <c r="A41" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="25" t="s">
         <v>173</v>
       </c>
       <c r="C41" s="2">
@@ -3388,7 +3450,7 @@
       <c r="A42" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="28" t="s">
         <v>133</v>
       </c>
       <c r="C42" s="2">
@@ -3420,7 +3482,7 @@
       <c r="A43" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="2">
@@ -3454,7 +3516,7 @@
       <c r="A44" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="28" t="s">
         <v>184</v>
       </c>
       <c r="C44" s="2">
@@ -3486,7 +3548,7 @@
       <c r="A45" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="28" t="s">
         <v>188</v>
       </c>
       <c r="C45" s="2">
@@ -3517,7 +3579,7 @@
       <c r="A46" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="28" t="s">
         <v>192</v>
       </c>
       <c r="C46" s="2">
@@ -3550,7 +3612,7 @@
       <c r="A47" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="25" t="s">
         <v>197</v>
       </c>
       <c r="C47" s="2">
@@ -3580,7 +3642,7 @@
       <c r="A48" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="25" t="s">
         <v>202</v>
       </c>
       <c r="C48" s="2">
@@ -3610,7 +3672,7 @@
       <c r="A49" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="25" t="s">
         <v>206</v>
       </c>
       <c r="C49" s="2">
@@ -3641,7 +3703,7 @@
       <c r="A50" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="25" t="s">
         <v>210</v>
       </c>
       <c r="C50" s="2">
@@ -3673,7 +3735,7 @@
       <c r="A51" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C51" s="2">
@@ -3704,7 +3766,7 @@
       <c r="A52" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C52" s="2">
@@ -3734,7 +3796,7 @@
       <c r="A53" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="28" t="s">
         <v>218</v>
       </c>
       <c r="C53" s="2">
@@ -3764,7 +3826,7 @@
       <c r="A54" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C54" s="2">
@@ -3795,7 +3857,7 @@
       <c r="A55" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C55" s="2">
@@ -3826,7 +3888,7 @@
       <c r="A56" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="2">
@@ -3859,7 +3921,7 @@
       <c r="A57" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="25" t="s">
         <v>230</v>
       </c>
       <c r="C57" s="2">
@@ -3892,7 +3954,7 @@
       <c r="A58" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="28" t="s">
         <v>202</v>
       </c>
       <c r="C58" s="2">
@@ -3925,7 +3987,7 @@
       <c r="A59" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="28" t="s">
         <v>237</v>
       </c>
       <c r="C59" s="2">
@@ -3960,7 +4022,7 @@
       <c r="A60" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="28" t="s">
         <v>241</v>
       </c>
       <c r="C60" s="2">
@@ -3995,7 +4057,7 @@
       <c r="A61" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="28" t="s">
         <v>245</v>
       </c>
       <c r="C61" s="2">
@@ -4028,7 +4090,7 @@
       <c r="A62" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="28" t="s">
         <v>133</v>
       </c>
       <c r="C62" s="2">
@@ -4059,7 +4121,7 @@
       <c r="A63" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="28" t="s">
         <v>253</v>
       </c>
       <c r="C63" s="2">
@@ -4090,7 +4152,7 @@
       <c r="A64" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="28" t="s">
         <v>257</v>
       </c>
       <c r="C64" s="2">
@@ -4121,7 +4183,7 @@
       <c r="A65" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="28" t="s">
         <v>261</v>
       </c>
       <c r="C65" s="2">
@@ -4152,7 +4214,7 @@
       <c r="A66" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="28" t="s">
         <v>265</v>
       </c>
       <c r="C66" s="2">
@@ -4187,7 +4249,7 @@
       <c r="A67" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="28" t="s">
         <v>146</v>
       </c>
       <c r="C67" s="2">
@@ -4220,7 +4282,7 @@
       <c r="A68" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="28" t="s">
         <v>273</v>
       </c>
       <c r="C68" s="2">
@@ -4253,7 +4315,7 @@
       <c r="A69" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="28" t="s">
         <v>277</v>
       </c>
       <c r="C69" s="2">
@@ -4284,7 +4346,7 @@
       <c r="A70" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="28" t="s">
         <v>146</v>
       </c>
       <c r="C70" s="2">
@@ -4317,7 +4379,7 @@
       <c r="A71" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="28" t="s">
         <v>284</v>
       </c>
       <c r="C71" s="2">
@@ -4348,14 +4410,14 @@
       <c r="A72" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>288</v>
+      <c r="B72" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="C72" s="2">
         <v>2002</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>79</v>
@@ -4364,7 +4426,7 @@
         <v>199</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2" t="s">
@@ -4379,23 +4441,23 @@
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B73" s="28" t="s">
         <v>291</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="C73" s="2">
         <v>1997</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E73" s="12"/>
       <c r="F73" s="30" t="s">
         <v>199</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2" t="s">
@@ -4410,16 +4472,16 @@
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B74" s="28" t="s">
         <v>295</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="C74" s="2">
         <v>1980</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E74" s="12"/>
       <c r="F74" s="10" t="s">
@@ -4441,25 +4503,25 @@
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B75" s="28" t="s">
         <v>298</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="C75" s="2">
         <v>2017</v>
       </c>
       <c r="D75" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="E75" s="12" t="s">
         <v>300</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>301</v>
       </c>
       <c r="F75" s="30" t="s">
         <v>199</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2" t="s">
@@ -4474,16 +4536,16 @@
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B76" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B76" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C76" s="2">
         <v>2004</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E76" s="12" t="s">
         <v>25</v>
@@ -4492,7 +4554,7 @@
         <v>11</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>12</v>
@@ -4506,22 +4568,22 @@
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B77" s="28" t="s">
         <v>306</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="C77" s="2">
         <v>2020</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F77" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>12</v>
@@ -4535,22 +4597,22 @@
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B78" s="28" t="s">
         <v>310</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="C78" s="2">
         <v>2017</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F78" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>12</v>
@@ -4564,22 +4626,22 @@
     </row>
     <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B79" s="28" t="s">
         <v>314</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="C79" s="2">
         <v>1991</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F79" s="30" t="s">
         <v>199</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>12</v>
@@ -4593,22 +4655,22 @@
     </row>
     <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="B80" s="28" t="s">
         <v>318</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>319</v>
       </c>
       <c r="C80" s="2">
         <v>1979</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F80" s="30" t="s">
         <v>199</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>12</v>
@@ -4622,22 +4684,22 @@
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="33" t="s">
-        <v>321</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
+      </c>
+      <c r="B81" s="28" t="s">
+        <v>322</v>
       </c>
       <c r="C81" s="2">
         <v>2022</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F81" s="30" t="s">
         <v>199</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>12</v>
@@ -4651,22 +4713,22 @@
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B82" s="28" t="s">
         <v>326</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="C82" s="2">
         <v>2020</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F82" s="30" t="s">
         <v>199</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>12</v>
@@ -4680,22 +4742,22 @@
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>323</v>
+        <v>329</v>
+      </c>
+      <c r="B83" s="28" t="s">
+        <v>322</v>
       </c>
       <c r="C83" s="2">
         <v>2014</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F83" s="30" t="s">
         <v>199</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>12</v>
@@ -4709,9 +4771,9 @@
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="33" t="s">
-        <v>333</v>
-      </c>
-      <c r="B84" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B84" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C84" s="2">
@@ -4724,7 +4786,7 @@
         <v>199</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>12</v>
@@ -4738,22 +4800,22 @@
     </row>
     <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="B85" s="28" t="s">
         <v>335</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>336</v>
       </c>
       <c r="C85" s="2">
         <v>1963</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>12</v>
@@ -4767,16 +4829,16 @@
     </row>
     <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B86" s="39" t="s">
         <v>339</v>
-      </c>
-      <c r="B86" s="37" t="s">
-        <v>340</v>
       </c>
       <c r="C86" s="2">
         <v>2024</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E86" s="12" t="s">
         <v>138</v>
@@ -4785,7 +4847,7 @@
         <v>11</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>12</v>
@@ -4799,16 +4861,16 @@
     </row>
     <row r="87" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B87" s="28" t="s">
         <v>342</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="C87" s="2">
         <v>2017</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E87" s="12" t="s">
         <v>138</v>
@@ -4817,7 +4879,7 @@
         <v>11</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>12</v>
@@ -4831,16 +4893,16 @@
     </row>
     <row r="88" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B88" s="28" t="s">
         <v>347</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="C88" s="2">
         <v>2024</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E88" s="12" t="s">
         <v>138</v>
@@ -4849,7 +4911,7 @@
         <v>11</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>12</v>
@@ -4863,22 +4925,22 @@
     </row>
     <row r="89" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B89" s="28" t="s">
         <v>351</v>
-      </c>
-      <c r="B89" s="28" t="s">
-        <v>352</v>
       </c>
       <c r="C89" s="2">
         <v>1986</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F89" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>12</v>
@@ -4892,22 +4954,22 @@
     </row>
     <row r="90" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="B90" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B90" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C90" s="2">
         <v>1995</v>
       </c>
       <c r="D90" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F90" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>12</v>
@@ -4921,22 +4983,22 @@
     </row>
     <row r="91" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B91" t="s">
         <v>358</v>
-      </c>
-      <c r="B91" t="s">
-        <v>359</v>
       </c>
       <c r="C91" s="2">
         <v>2009</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F91" s="30" t="s">
         <v>199</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>12</v>
@@ -4950,30 +5012,207 @@
     </row>
     <row r="92" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>296</v>
+        <v>362</v>
+      </c>
+      <c r="B92" s="28" t="s">
+        <v>295</v>
       </c>
       <c r="C92" s="2">
         <v>1998</v>
       </c>
       <c r="D92" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="F92" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="F92" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K92" s="2" t="s">
+      <c r="B93" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="C93" s="2">
+        <v>1981</v>
+      </c>
+      <c r="D93" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="F93" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B94" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="C94" s="2">
+        <v>2008</v>
+      </c>
+      <c r="D94" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="F94" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B95" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="C95" s="2">
+        <v>2002</v>
+      </c>
+      <c r="D95" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="F95" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B96" t="s">
+        <v>377</v>
+      </c>
+      <c r="C96" s="2">
+        <v>1988</v>
+      </c>
+      <c r="D96" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F96" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B97" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="C97">
+        <v>2024</v>
+      </c>
+      <c r="D97" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="F97" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B98" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C98" s="2">
+        <v>2008</v>
+      </c>
+      <c r="D98" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K98" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correction in reference inventory
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4522CF-6CDB-004A-A33F-AD0378C4715B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BE1555-FFE1-8B45-9D97-D7D433D47659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29460" yWindow="500" windowWidth="29100" windowHeight="16920" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="384">
   <si>
     <t>Paper Title</t>
   </si>
@@ -673,12 +673,6 @@
     <t>Handicap principle</t>
   </si>
   <si>
-    <t>Julien</t>
-  </si>
-  <si>
-    <t>Julien???</t>
-  </si>
-  <si>
     <t>Bigger is not always better: viability selection on body mass varies across life stages in a hibernating mammal</t>
   </si>
   <si>
@@ -1313,7 +1307,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1428,12 +1422,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="6"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1617,7 +1605,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1710,17 +1698,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2069,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E69" workbookViewId="0">
-      <selection activeCell="K98" sqref="K98"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2091,16 +2076,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -2127,7 +2112,7 @@
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="28" t="s">
@@ -2199,7 +2184,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="28" t="s">
@@ -2230,7 +2215,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="28" t="s">
@@ -2263,7 +2248,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -2463,7 +2448,7 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="33" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -2497,7 +2482,7 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="33" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="28" t="s">
@@ -2531,7 +2516,7 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B14" s="28" t="s">
@@ -2565,7 +2550,7 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>63</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -2600,7 +2585,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>69</v>
       </c>
       <c r="B16" s="28"/>
@@ -2622,8 +2607,8 @@
       <c r="I16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="29" t="s">
-        <v>181</v>
+      <c r="J16" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>12</v>
@@ -2661,7 +2646,7 @@
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>85</v>
@@ -2690,7 +2675,7 @@
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="33" t="s">
         <v>84</v>
       </c>
       <c r="B19" s="28" t="s">
@@ -2714,7 +2699,7 @@
       <c r="J19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="36" t="s">
+      <c r="K19" s="35" t="s">
         <v>13</v>
       </c>
       <c r="L19" s="2"/>
@@ -2723,20 +2708,20 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="37" t="s">
         <v>92</v>
       </c>
       <c r="C20" s="8">
         <v>1965</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="37" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -2769,7 +2754,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>96</v>
       </c>
       <c r="B21" s="28" t="s">
@@ -2810,7 +2795,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="32" t="s">
         <v>99</v>
       </c>
       <c r="B22" s="28" t="s">
@@ -2846,7 +2831,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="32" t="s">
         <v>101</v>
       </c>
       <c r="B23" s="28" t="s">
@@ -2912,7 +2897,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="33" t="s">
         <v>108</v>
       </c>
       <c r="B25" s="28" t="s">
@@ -2979,7 +2964,7 @@
       </c>
       <c r="N26" s="19">
         <f>COUNTIF(J:J, "no")</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3001,8 +2986,8 @@
       <c r="I27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="29" t="s">
-        <v>181</v>
+      <c r="J27" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>12</v>
@@ -3068,7 +3053,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="33" t="s">
         <v>128</v>
       </c>
       <c r="B30" s="28" t="s">
@@ -3199,7 +3184,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="33" t="s">
         <v>145</v>
       </c>
       <c r="B34" s="28" t="s">
@@ -3232,7 +3217,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="33" t="s">
         <v>151</v>
       </c>
       <c r="B35" s="28" t="s">
@@ -3266,7 +3251,7 @@
       <c r="L35" s="8"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="33" t="s">
         <v>152</v>
       </c>
       <c r="B36" s="28" t="s">
@@ -3447,7 +3432,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="33" t="s">
         <v>175</v>
       </c>
       <c r="B42" s="28" t="s">
@@ -3479,7 +3464,7 @@
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="33" t="s">
         <v>178</v>
       </c>
       <c r="B43" s="28" t="s">
@@ -3504,33 +3489,33 @@
       <c r="I43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J43" s="29" t="s">
+      <c r="J43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B44" s="28" t="s">
         <v>182</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>184</v>
       </c>
       <c r="C44" s="2">
         <v>2021</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="s">
@@ -3545,24 +3530,24 @@
       <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="34" t="s">
-        <v>187</v>
+      <c r="A45" s="33" t="s">
+        <v>185</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C45" s="2">
         <v>2003</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="30" t="s">
-        <v>199</v>
+      <c r="F45" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2" t="s">
@@ -3576,27 +3561,27 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="34" t="s">
-        <v>191</v>
+      <c r="A46" s="33" t="s">
+        <v>189</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C46" s="2">
         <v>2010</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>12</v>
@@ -3610,22 +3595,22 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C47" s="2">
         <v>1989</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="2" t="s">
@@ -3640,23 +3625,23 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C48" s="2">
         <v>2001</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>12</v>
@@ -3670,23 +3655,23 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C49" s="2">
         <v>2010</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="2" t="s">
@@ -3701,23 +3686,23 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C50" s="2">
         <v>2007</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="2" t="s">
@@ -3733,7 +3718,7 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B51" s="25" t="s">
         <v>64</v>
@@ -3742,14 +3727,14 @@
         <v>2007</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="2" t="s">
@@ -3764,7 +3749,7 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B52" s="28" t="s">
         <v>41</v>
@@ -3773,14 +3758,14 @@
         <v>2008</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>12</v>
@@ -3794,22 +3779,22 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C53" s="2">
         <v>2011</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2" t="s">
@@ -3824,7 +3809,7 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B54" s="28" t="s">
         <v>41</v>
@@ -3833,14 +3818,14 @@
         <v>2002</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H54" s="8"/>
       <c r="I54" s="2" t="s">
@@ -3854,8 +3839,8 @@
       </c>
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="33" t="s">
-        <v>224</v>
+      <c r="A55" s="32" t="s">
+        <v>222</v>
       </c>
       <c r="B55" s="28" t="s">
         <v>41</v>
@@ -3864,14 +3849,14 @@
         <v>2013</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2" t="s">
@@ -3885,8 +3870,8 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="34" t="s">
-        <v>226</v>
+      <c r="A56" s="33" t="s">
+        <v>224</v>
       </c>
       <c r="B56" s="28" t="s">
         <v>31</v>
@@ -3895,7 +3880,7 @@
         <v>1992</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>25</v>
@@ -3904,14 +3889,14 @@
         <v>13</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J56" s="29" t="s">
-        <v>182</v>
+      <c r="J56" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>12</v>
@@ -3919,32 +3904,32 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C57" s="2">
         <v>2023</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="E57" s="31" t="s">
-        <v>232</v>
+        <v>229</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>230</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J57" s="29" t="s">
-        <v>182</v>
+      <c r="J57" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>12</v>
@@ -3952,25 +3937,25 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C58" s="2">
         <v>2003</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F58" s="30" t="s">
-        <v>199</v>
+      <c r="F58" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="2" t="s">
@@ -3985,16 +3970,16 @@
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C59" s="2">
         <v>2024</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>138</v>
@@ -4003,10 +3988,10 @@
         <v>11</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>12</v>
@@ -4020,16 +4005,16 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C60" s="2">
         <v>2024</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>138</v>
@@ -4038,10 +4023,10 @@
         <v>11</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>12</v>
@@ -4055,16 +4040,16 @@
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C61" s="2">
         <v>2006</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>138</v>
@@ -4073,7 +4058,7 @@
         <v>11</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2" t="s">
@@ -4087,8 +4072,8 @@
       </c>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="34" t="s">
-        <v>249</v>
+      <c r="A62" s="33" t="s">
+        <v>247</v>
       </c>
       <c r="B62" s="28" t="s">
         <v>133</v>
@@ -4097,14 +4082,14 @@
         <v>2010</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E62" s="2"/>
-      <c r="F62" s="30" t="s">
-        <v>199</v>
+      <c r="F62" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2" t="s">
@@ -4118,24 +4103,24 @@
       </c>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="34" t="s">
-        <v>252</v>
+      <c r="A63" s="33" t="s">
+        <v>250</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C63" s="2">
         <v>1966</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2" t="s">
@@ -4149,24 +4134,24 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="34" t="s">
-        <v>256</v>
+      <c r="A64" s="33" t="s">
+        <v>254</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C64" s="2">
         <v>2010</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2" t="s">
@@ -4180,24 +4165,24 @@
       </c>
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="34" t="s">
-        <v>260</v>
+      <c r="A65" s="33" t="s">
+        <v>258</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C65" s="2">
         <v>2012</v>
       </c>
       <c r="D65" s="28" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E65" s="2"/>
-      <c r="F65" s="32" t="s">
-        <v>263</v>
+      <c r="F65" s="31" t="s">
+        <v>261</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2" t="s">
@@ -4212,16 +4197,16 @@
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C66" s="2">
         <v>2023</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>138</v>
@@ -4230,10 +4215,10 @@
         <v>11</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>12</v>
@@ -4247,7 +4232,7 @@
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B67" s="28" t="s">
         <v>146</v>
@@ -4256,7 +4241,7 @@
         <v>2017</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>138</v>
@@ -4265,7 +4250,7 @@
         <v>11</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2" t="s">
@@ -4280,16 +4265,16 @@
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C68" s="2">
         <v>2001</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>25</v>
@@ -4298,7 +4283,7 @@
         <v>11</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2" t="s">
@@ -4313,23 +4298,23 @@
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C69" s="2">
         <v>2010</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E69" s="12"/>
-      <c r="F69" s="30" t="s">
-        <v>199</v>
+      <c r="F69" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2" t="s">
@@ -4343,8 +4328,8 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="34" t="s">
-        <v>280</v>
+      <c r="A70" s="33" t="s">
+        <v>278</v>
       </c>
       <c r="B70" s="28" t="s">
         <v>146</v>
@@ -4353,7 +4338,7 @@
         <v>2016</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>138</v>
@@ -4362,7 +4347,7 @@
         <v>11</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2" t="s">
@@ -4377,23 +4362,23 @@
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C71" s="2">
         <v>2012</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E71" s="12"/>
-      <c r="F71" s="30" t="s">
-        <v>199</v>
+      <c r="F71" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2" t="s">
@@ -4408,7 +4393,7 @@
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B72" s="28" t="s">
         <v>11</v>
@@ -4417,16 +4402,16 @@
         <v>2002</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F72" s="30" t="s">
-        <v>199</v>
+      <c r="F72" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2" t="s">
@@ -4441,23 +4426,23 @@
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B73" s="28" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C73" s="2">
         <v>1997</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E73" s="12"/>
-      <c r="F73" s="30" t="s">
-        <v>199</v>
+      <c r="F73" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2" t="s">
@@ -4472,23 +4457,23 @@
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C74" s="2">
         <v>1980</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E74" s="12"/>
       <c r="F74" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2" t="s">
@@ -4503,25 +4488,25 @@
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C75" s="2">
         <v>2017</v>
       </c>
       <c r="D75" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="F75" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G75" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="F75" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2" t="s">
@@ -4536,7 +4521,7 @@
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B76" s="28" t="s">
         <v>23</v>
@@ -4545,7 +4530,7 @@
         <v>2004</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E76" s="12" t="s">
         <v>25</v>
@@ -4554,7 +4539,7 @@
         <v>11</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>12</v>
@@ -4568,22 +4553,22 @@
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C77" s="2">
         <v>2020</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F77" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>12</v>
@@ -4597,22 +4582,22 @@
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C78" s="2">
         <v>2017</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F78" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>12</v>
@@ -4626,51 +4611,51 @@
     </row>
     <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B79" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C79" s="2">
         <v>1991</v>
       </c>
       <c r="D79" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="F79" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="F79" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="G79" s="2" t="s">
+      <c r="B80" s="28" t="s">
         <v>316</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="B80" s="28" t="s">
-        <v>318</v>
       </c>
       <c r="C80" s="2">
         <v>1979</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>319</v>
-      </c>
-      <c r="F80" s="30" t="s">
-        <v>199</v>
+        <v>317</v>
+      </c>
+      <c r="F80" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>12</v>
@@ -4683,23 +4668,23 @@
       </c>
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="33" t="s">
+      <c r="A81" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="B81" s="28" t="s">
         <v>320</v>
-      </c>
-      <c r="B81" s="28" t="s">
-        <v>322</v>
       </c>
       <c r="C81" s="2">
         <v>2022</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>323</v>
-      </c>
-      <c r="F81" s="30" t="s">
-        <v>199</v>
+        <v>321</v>
+      </c>
+      <c r="F81" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>12</v>
@@ -4713,22 +4698,22 @@
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B82" s="28" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C82" s="2">
         <v>2020</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>327</v>
-      </c>
-      <c r="F82" s="30" t="s">
-        <v>199</v>
+        <v>325</v>
+      </c>
+      <c r="F82" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>12</v>
@@ -4742,36 +4727,36 @@
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B83" s="28" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C83" s="2">
         <v>2014</v>
       </c>
       <c r="D83" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="F83" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="32" t="s">
         <v>330</v>
-      </c>
-      <c r="F83" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J83" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="33" t="s">
-        <v>332</v>
       </c>
       <c r="B84" s="28" t="s">
         <v>41</v>
@@ -4780,42 +4765,42 @@
         <v>2005</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="F84" s="30" t="s">
-        <v>199</v>
+        <v>272</v>
+      </c>
+      <c r="F84" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G84" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="B85" s="28" t="s">
         <v>333</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="33" t="s">
-        <v>334</v>
-      </c>
-      <c r="B85" s="28" t="s">
-        <v>335</v>
       </c>
       <c r="C85" s="2">
         <v>1963</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>12</v>
@@ -4829,16 +4814,16 @@
     </row>
     <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="B86" s="39" t="s">
-        <v>339</v>
+        <v>336</v>
+      </c>
+      <c r="B86" s="38" t="s">
+        <v>337</v>
       </c>
       <c r="C86" s="2">
         <v>2024</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E86" s="12" t="s">
         <v>138</v>
@@ -4847,7 +4832,7 @@
         <v>11</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>12</v>
@@ -4861,16 +4846,16 @@
     </row>
     <row r="87" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C87" s="2">
         <v>2017</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E87" s="12" t="s">
         <v>138</v>
@@ -4879,7 +4864,7 @@
         <v>11</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>12</v>
@@ -4893,16 +4878,16 @@
     </row>
     <row r="88" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C88" s="2">
         <v>2024</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E88" s="12" t="s">
         <v>138</v>
@@ -4911,7 +4896,7 @@
         <v>11</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>12</v>
@@ -4925,22 +4910,22 @@
     </row>
     <row r="89" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C89" s="2">
         <v>1986</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F89" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>12</v>
@@ -4954,7 +4939,7 @@
     </row>
     <row r="90" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B90" s="28" t="s">
         <v>41</v>
@@ -4963,13 +4948,13 @@
         <v>1995</v>
       </c>
       <c r="D90" s="28" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F90" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>12</v>
@@ -4983,22 +4968,22 @@
     </row>
     <row r="91" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B91" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C91" s="2">
         <v>2009</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>359</v>
-      </c>
-      <c r="F91" s="30" t="s">
-        <v>199</v>
+        <v>357</v>
+      </c>
+      <c r="F91" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>12</v>
@@ -5012,22 +4997,22 @@
     </row>
     <row r="92" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C92" s="2">
         <v>1998</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F92" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I92" s="2" t="s">
         <v>12</v>
@@ -5041,22 +5026,22 @@
     </row>
     <row r="93" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C93" s="2">
         <v>1981</v>
       </c>
       <c r="D93" s="28" t="s">
-        <v>366</v>
-      </c>
-      <c r="F93" s="30" t="s">
-        <v>199</v>
+        <v>364</v>
+      </c>
+      <c r="F93" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>12</v>
@@ -5070,22 +5055,22 @@
     </row>
     <row r="94" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C94" s="2">
         <v>2008</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>370</v>
-      </c>
-      <c r="F94" s="30" t="s">
-        <v>199</v>
+        <v>368</v>
+      </c>
+      <c r="F94" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>12</v>
@@ -5099,22 +5084,22 @@
     </row>
     <row r="95" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C95" s="2">
         <v>2002</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>374</v>
-      </c>
-      <c r="F95" s="30" t="s">
-        <v>199</v>
+        <v>372</v>
+      </c>
+      <c r="F95" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>12</v>
@@ -5128,16 +5113,16 @@
     </row>
     <row r="96" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B96" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C96" s="2">
         <v>1988</v>
       </c>
       <c r="D96" s="28" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>79</v>
@@ -5146,7 +5131,7 @@
         <v>13</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>12</v>
@@ -5160,22 +5145,22 @@
     </row>
     <row r="97" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C97">
         <v>2024</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>382</v>
-      </c>
-      <c r="F97" s="30" t="s">
-        <v>199</v>
+        <v>380</v>
+      </c>
+      <c r="F97" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>12</v>
@@ -5189,7 +5174,7 @@
     </row>
     <row r="98" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B98" s="28" t="s">
         <v>133</v>
@@ -5204,7 +5189,7 @@
         <v>13</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
remake - chapter 3 & 4
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BE1555-FFE1-8B45-9D97-D7D433D47659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC338839-7BC9-D24B-90C7-710EF39323FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="405">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1301,6 +1301,69 @@
   </si>
   <si>
     <t>Estimating evolutionary parameters when viability selection is operating</t>
+  </si>
+  <si>
+    <t>Integrating animal temperament within ecology and evolution</t>
+  </si>
+  <si>
+    <t>Réale et al.</t>
+  </si>
+  <si>
+    <t>THE BIG FIVES (personality)</t>
+  </si>
+  <si>
+    <t>Animal personalities: consequences for ecology and evolution</t>
+  </si>
+  <si>
+    <t>Wolf &amp; Weissing</t>
+  </si>
+  <si>
+    <t>Impact of personality on eco-evo (e.g., pop dynamic) REVIEW</t>
+  </si>
+  <si>
+    <t>The development of animal personality: relevance, concepts and perspectives</t>
+  </si>
+  <si>
+    <t>Stamps &amp; Groothuis</t>
+  </si>
+  <si>
+    <t>impact of age on personnality</t>
+  </si>
+  <si>
+    <t>Animal social networks</t>
+  </si>
+  <si>
+    <t>Krause et al.</t>
+  </si>
+  <si>
+    <t>Constructing, conducting and interpreting animal social network analysis</t>
+  </si>
+  <si>
+    <t>Farine and Whitehead</t>
+  </si>
+  <si>
+    <t>SNA</t>
+  </si>
+  <si>
+    <t>The Evolution of Bet Hedging in Response to Local Ecological Conditions</t>
+  </si>
+  <si>
+    <t>Rajon, Desouhant, Chevalier, Débias, Menu</t>
+  </si>
+  <si>
+    <t>bet-hedging</t>
+  </si>
+  <si>
+    <t>Environmental unpredicatbility and offspring size: conservative versus diversified bet-hedging</t>
+  </si>
+  <si>
+    <t>Evolutionary Ecology Research</t>
+  </si>
+  <si>
+    <t>Einum and flemming</t>
+  </si>
+  <si>
+    <t>Conservative bet-hedging =&gt; bigger to buffer unpredictability</t>
   </si>
 </sst>
 </file>
@@ -2052,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" topLeftCell="E84" workbookViewId="0">
+      <selection activeCell="K105" sqref="K105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2708,7 +2771,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2750,7 +2813,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2784,7 +2847,7 @@
       </c>
       <c r="N21" s="17">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O21" s="18" t="s">
         <v>16</v>
@@ -2827,7 +2890,7 @@
       </c>
       <c r="N22" s="21">
         <f>COUNTIF(F:F, "no")</f>
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2893,7 +2956,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5198,6 +5261,209 @@
         <v>12</v>
       </c>
       <c r="K98" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B99" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C99" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D99" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="F99" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B100" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C100" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D100" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="F100" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C101" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D101" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="F101" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B102" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C102" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D102" s="28" t="s">
+        <v>394</v>
+      </c>
+      <c r="F102" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K102" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B103" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C103" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D103" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F103" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K103" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B104" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="C104" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D104" s="28" t="s">
+        <v>399</v>
+      </c>
+      <c r="F104" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B105" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="C105" s="2">
+        <v>2004</v>
+      </c>
+      <c r="D105" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="F105" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K105" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Work in progress - bet hedging
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC338839-7BC9-D24B-90C7-710EF39323FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D0C64C-BA80-5642-BDC7-F52CF49427E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="48680" yWindow="680" windowWidth="18980" windowHeight="19620" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="408">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1364,6 +1364,15 @@
   </si>
   <si>
     <t>Conservative bet-hedging =&gt; bigger to buffer unpredictability</t>
+  </si>
+  <si>
+    <t>Hedging one's evolutionary bets, revisited</t>
+  </si>
+  <si>
+    <t>Philipi &amp; Seger</t>
+  </si>
+  <si>
+    <t>Bet-hedging</t>
   </si>
 </sst>
 </file>
@@ -2115,10 +2124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P105"/>
+  <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E84" workbookViewId="0">
-      <selection activeCell="K105" sqref="K105"/>
+    <sheetView tabSelected="1" topLeftCell="H84" workbookViewId="0">
+      <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2771,7 +2780,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2813,7 +2822,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2956,7 +2965,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5464,6 +5473,35 @@
         <v>12</v>
       </c>
       <c r="K105" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B106" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106" s="2">
+        <v>1989</v>
+      </c>
+      <c r="D106" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="F106" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K106" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reshaping LHT and role of body mass paragraphs + citations (work in progress
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D0C64C-BA80-5642-BDC7-F52CF49427E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4EE0E9-63FE-3143-B67A-624D4D193D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48680" yWindow="680" windowWidth="18980" windowHeight="19620" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="48680" yWindow="680" windowWidth="18980" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="429">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1373,6 +1373,69 @@
   </si>
   <si>
     <t>Bet-hedging</t>
+  </si>
+  <si>
+    <t>The Misuse of BLUP in Ecology and Evolution</t>
+  </si>
+  <si>
+    <t>BLUPs</t>
+  </si>
+  <si>
+    <t>Martin &amp; Pelletier</t>
+  </si>
+  <si>
+    <t>Measuring growth patterns in the field: effects of sampling regime and methods on standardized estimates</t>
+  </si>
+  <si>
+    <t>Organisms as Ecosystem Engineers</t>
+  </si>
+  <si>
+    <t>Jones, Lawton &amp; Shachak</t>
+  </si>
+  <si>
+    <t>Concept of engineers species and example of Beavers</t>
+  </si>
+  <si>
+    <t>The measurement of selection on correlated characters</t>
+  </si>
+  <si>
+    <t>Lande &amp; Arnold</t>
+  </si>
+  <si>
+    <t>Behavioral types as predictors of survival in Trinidadian guppies (Poecilia reticulata)</t>
+  </si>
+  <si>
+    <t>Behavioral Ecology</t>
+  </si>
+  <si>
+    <t>Smith et Blumstein</t>
+  </si>
+  <si>
+    <t>bold, active and exploratory guppies survive longer when exposed to predators</t>
+  </si>
+  <si>
+    <t>Impact of Body Reserves on Energy Expenditure, Water Flux, and Mating Success in Breeding Male Northern Elephant Seals</t>
+  </si>
+  <si>
+    <t>Physiological and Biochemical Zoology</t>
+  </si>
+  <si>
+    <t>Crocker, Houser &amp; Webb</t>
+  </si>
+  <si>
+    <t>Bigger elephant seals have a better mating success</t>
+  </si>
+  <si>
+    <t>Link between winter body mass variation and reproductive success in female northern moose (Alces alces)</t>
+  </si>
+  <si>
+    <t>Milner et al.</t>
+  </si>
+  <si>
+    <t>Oecologia</t>
+  </si>
+  <si>
+    <t>Reproductive success and failure: the role of winter body mass in reproductive allocation in Norwegian moose</t>
   </si>
 </sst>
 </file>
@@ -2124,10 +2187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P106"/>
+  <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H84" workbookViewId="0">
-      <selection activeCell="K106" sqref="K106"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2780,7 +2843,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2822,7 +2885,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2856,7 +2919,7 @@
       </c>
       <c r="N21" s="17">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O21" s="18" t="s">
         <v>16</v>
@@ -2965,7 +3028,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2997,8 +3060,8 @@
       <c r="J25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="2" t="s">
-        <v>12</v>
+      <c r="K25" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="L25" s="2"/>
     </row>
@@ -5502,6 +5565,203 @@
         <v>12</v>
       </c>
       <c r="K106" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B107" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="C107" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D107" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="F107" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B108" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="C108" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D108" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="F108" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B109" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C109" s="2">
+        <v>1994</v>
+      </c>
+      <c r="D109" s="28" t="s">
+        <v>413</v>
+      </c>
+      <c r="F109" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B110" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C110" s="2">
+        <v>1983</v>
+      </c>
+      <c r="D110" s="28" t="s">
+        <v>416</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K110" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B111" s="28" t="s">
+        <v>418</v>
+      </c>
+      <c r="C111" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D111" s="28" t="s">
+        <v>419</v>
+      </c>
+      <c r="F111" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B112" s="28" t="s">
+        <v>422</v>
+      </c>
+      <c r="C112" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D112" s="28" t="s">
+        <v>423</v>
+      </c>
+      <c r="F112" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B113" s="28" t="s">
+        <v>427</v>
+      </c>
+      <c r="C113" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D113" s="28" t="s">
+        <v>426</v>
+      </c>
+      <c r="F113" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K113" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding marmot illustration + adressing comments
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA5141A-9C7C-0A43-A759-9B9361DEE4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4104A6-A038-3B49-A175-EFE962569D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48680" yWindow="680" windowWidth="18980" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="436">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1445,6 +1445,18 @@
   </si>
   <si>
     <t>Body condition and time of nesting impact survival probability in 3 species of ducks</t>
+  </si>
+  <si>
+    <t>The Relationship Between Body Mass and Survival of Wintering Canvasbacks</t>
+  </si>
+  <si>
+    <t>The Auk</t>
+  </si>
+  <si>
+    <t>Haramis et al.</t>
+  </si>
+  <si>
+    <t>Individuals with heavier early-winter body mass had better overall survival probability in adults males Canvasbacks *Aythya valisineria*</t>
   </si>
 </sst>
 </file>
@@ -2198,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="H68" workbookViewId="0">
+      <selection activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2852,7 +2864,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2894,7 +2906,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3037,7 +3049,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5803,8 +5815,34 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G115" s="2"/>
+    <row r="115" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B115" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="C115" s="2">
+        <v>1986</v>
+      </c>
+      <c r="D115" s="28" t="s">
+        <v>434</v>
+      </c>
+      <c r="F115" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K115" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
paragraph "the role of body mass"
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4104A6-A038-3B49-A175-EFE962569D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B416E3B-917F-7C4A-8EB3-D5D46085C623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48680" yWindow="680" windowWidth="18980" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="443">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1457,6 +1457,27 @@
   </si>
   <si>
     <t>Individuals with heavier early-winter body mass had better overall survival probability in adults males Canvasbacks *Aythya valisineria*</t>
+  </si>
+  <si>
+    <t>Darveau et al.</t>
+  </si>
+  <si>
+    <t>Allometric cascade as a unifyind principle of body mass effects on metabolism</t>
+  </si>
+  <si>
+    <t>Body mass effect on metabolic rate (allometric relation)</t>
+  </si>
+  <si>
+    <t>Max metabolic rate ~ body mass (allometric) =&gt; R^2 = 0.96</t>
+  </si>
+  <si>
+    <t>Weibel et al.</t>
+  </si>
+  <si>
+    <t>Respiratory Physiology &amp; Neurobiology</t>
+  </si>
+  <si>
+    <t>Allometric scaling of maximal metabolic rate in mammals: muscle aerobic capacity as determinant factor</t>
   </si>
 </sst>
 </file>
@@ -2208,10 +2229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H68" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2864,7 +2885,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2906,7 +2927,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3049,7 +3070,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5841,6 +5862,64 @@
         <v>12</v>
       </c>
       <c r="K115" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B116" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C116" s="2">
+        <v>2002</v>
+      </c>
+      <c r="D116" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="F116" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B117" s="28" t="s">
+        <v>441</v>
+      </c>
+      <c r="C117" s="2">
+        <v>2004</v>
+      </c>
+      <c r="D117" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="F117" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K117" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ref bighorn sheep horn size
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B416E3B-917F-7C4A-8EB3-D5D46085C623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D965F297-A666-5948-9357-3C5F77DD0C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48680" yWindow="680" windowWidth="18980" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="446">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1478,6 +1478,15 @@
   </si>
   <si>
     <t>Allometric scaling of maximal metabolic rate in mammals: muscle aerobic capacity as determinant factor</t>
+  </si>
+  <si>
+    <t>Ewe are what ewe wear: bigger horns, better ewes and the potential consequence of trophy hunting on female fitness in bighorn sheep</t>
+  </si>
+  <si>
+    <t>Deakin et al.</t>
+  </si>
+  <si>
+    <t>Correlation horn size at 2 y.o. and LRS</t>
   </si>
 </sst>
 </file>
@@ -2229,10 +2238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P117"/>
+  <dimension ref="A1:P118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="H80" workbookViewId="0">
+      <selection activeCell="I119" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2885,7 +2894,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2927,7 +2936,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3070,7 +3079,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5920,6 +5929,35 @@
         <v>12</v>
       </c>
       <c r="K117" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B118" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C118" s="2">
+        <v>2022</v>
+      </c>
+      <c r="D118" s="28" t="s">
+        <v>444</v>
+      </c>
+      <c r="F118" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K118" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Body mass and competition
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D965F297-A666-5948-9357-3C5F77DD0C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2B4728-BCE5-C547-9812-2BB4A133509A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48680" yWindow="680" windowWidth="18980" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="458">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1487,6 +1487,42 @@
   </si>
   <si>
     <t>Correlation horn size at 2 y.o. and LRS</t>
+  </si>
+  <si>
+    <t>Assessment of energy reserves by damselflies engaged in aerial contests for mating territories</t>
+  </si>
+  <si>
+    <t>Marden &amp; Rollins</t>
+  </si>
+  <si>
+    <t>males *Calopteryx maculata* with more fat win contests for mating territory in 88 % of cases</t>
+  </si>
+  <si>
+    <t>Female competition and its evolutionary consequences in mammals</t>
+  </si>
+  <si>
+    <t>Stockley &amp; Bro-Jørgensen</t>
+  </si>
+  <si>
+    <t>"there is evidence that female dominance may often be correlated with age or body size"; "larger females consistently dominate" (e.g., feral ponies and african elephants)</t>
+  </si>
+  <si>
+    <t>Dominance, aggression frequencies and modes of aggressive competition in feral pony mares</t>
+  </si>
+  <si>
+    <t>Rutberg &amp; Greenberg</t>
+  </si>
+  <si>
+    <t>Older and Larger Equus caballus are dominant</t>
+  </si>
+  <si>
+    <t>Older and Larger Loxodonta africana are dominant</t>
+  </si>
+  <si>
+    <t>Dominance rank relationships among wild female African elephants, Loxodonta africana</t>
+  </si>
+  <si>
+    <t>Archie et al.</t>
   </si>
 </sst>
 </file>
@@ -2238,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P118"/>
+  <dimension ref="A1:P122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H80" workbookViewId="0">
-      <selection activeCell="I119" sqref="I119"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2894,7 +2930,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2936,7 +2972,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3079,7 +3115,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5958,6 +5994,122 @@
         <v>12</v>
       </c>
       <c r="K118" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B119" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C119" s="2">
+        <v>1994</v>
+      </c>
+      <c r="D119" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="F119" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="B120" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C120" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D120" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="F120" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G120" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B121" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C121" s="2">
+        <v>1990</v>
+      </c>
+      <c r="D121" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="F121" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B122" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C122" s="2">
+        <v>2006</v>
+      </c>
+      <c r="D122" s="28" t="s">
+        <v>457</v>
+      </c>
+      <c r="F122" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="I122" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J122" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K122" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
life history trait section
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174FF2E0-8571-6B41-92B6-91B384BF818B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E495B6-487D-3947-8012-9E5808389576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29540" yWindow="680" windowWidth="18980" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="485">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1201,9 +1201,6 @@
     <t>Advances in the study of behavior, vol. 16 (Elsevier)</t>
   </si>
   <si>
-    <t>Yedenberg &amp; Dill</t>
-  </si>
-  <si>
     <t>FID</t>
   </si>
   <si>
@@ -1234,9 +1231,6 @@
     <t>Mass‐ and Density‐Dependent Reproductive Success and Reproductive Costs in a Capital Breeder</t>
   </si>
   <si>
-    <t>Fest-bianchet, Gaillard, Jorgenson</t>
-  </si>
-  <si>
     <t>The role of body mass in thermoregulation</t>
   </si>
   <si>
@@ -1367,9 +1361,6 @@
   </si>
   <si>
     <t>Hedging one's evolutionary bets, revisited</t>
-  </si>
-  <si>
-    <t>Philipi &amp; Seger</t>
   </si>
   <si>
     <t>Bet-hedging</t>
@@ -1596,12 +1587,42 @@
   <si>
     <t>3 conditions for evolution (Phenotypic variation; differential fitness; heritable fitness)</t>
   </si>
+  <si>
+    <t>Festa-bianchet, Gaillard, Jorgenson</t>
+  </si>
+  <si>
+    <t>Philips &amp; Seger</t>
+  </si>
+  <si>
+    <t>Ydenberg &amp; Dill</t>
+  </si>
+  <si>
+    <t>Towards robust evolutionary inference with integral projection models</t>
+  </si>
+  <si>
+    <t>Janeiro, Coltman, Festa-Bianchet, Pelletier &amp; Morissey</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>IPM doesn't model evolutionary signals and will almost allways conclude to the absence of evolution (explaining phenotyping shift by phenotypic plasticity mostly)</t>
+  </si>
+  <si>
+    <t>Evolution of adult size depends on genetic variance in growth trajectories: a comment on analyses of evolutionary dynamics using integral projection models</t>
+  </si>
+  <si>
+    <t>Mehtods in Ecology and Evolution</t>
+  </si>
+  <si>
+    <t>Chevin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1767,6 +1788,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF156082"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1906,7 +1947,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2017,6 +2058,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2353,12 +2403,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P128"/>
+  <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="K128" sqref="K128"/>
+      <selection pane="bottomLeft" activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3011,7 +3061,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3053,7 +3103,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3087,7 +3137,7 @@
       </c>
       <c r="N21" s="17">
         <f>COUNTIF(F:F, "yes")</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O21" s="18" t="s">
         <v>16</v>
@@ -3196,7 +3246,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5222,13 +5272,13 @@
         <v>1986</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>350</v>
+        <v>477</v>
       </c>
       <c r="F89" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>12</v>
@@ -5242,7 +5292,7 @@
     </row>
     <row r="90" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B90" s="28" t="s">
         <v>41</v>
@@ -5251,13 +5301,13 @@
         <v>1995</v>
       </c>
       <c r="D90" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F90" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>12</v>
@@ -5271,22 +5321,22 @@
     </row>
     <row r="91" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B91" t="s">
         <v>355</v>
-      </c>
-      <c r="B91" t="s">
-        <v>356</v>
       </c>
       <c r="C91" s="2">
         <v>2009</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F91" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>12</v>
@@ -5300,7 +5350,7 @@
     </row>
     <row r="92" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B92" s="28" t="s">
         <v>293</v>
@@ -5309,13 +5359,13 @@
         <v>1998</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>361</v>
+        <v>475</v>
       </c>
       <c r="F92" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I92" s="2" t="s">
         <v>12</v>
@@ -5329,22 +5379,22 @@
     </row>
     <row r="93" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C93" s="2">
         <v>1981</v>
       </c>
       <c r="D93" s="28" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F93" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>12</v>
@@ -5358,22 +5408,22 @@
     </row>
     <row r="94" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C94" s="2">
         <v>2008</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F94" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>12</v>
@@ -5387,22 +5437,22 @@
     </row>
     <row r="95" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C95" s="2">
         <v>2002</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F95" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>12</v>
@@ -5416,16 +5466,16 @@
     </row>
     <row r="96" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B96" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C96" s="2">
         <v>1988</v>
       </c>
       <c r="D96" s="28" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>79</v>
@@ -5434,7 +5484,7 @@
         <v>13</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>12</v>
@@ -5448,22 +5498,22 @@
     </row>
     <row r="97" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C97">
         <v>2024</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F97" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>12</v>
@@ -5477,7 +5527,7 @@
     </row>
     <row r="98" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B98" s="28" t="s">
         <v>133</v>
@@ -5492,7 +5542,7 @@
         <v>13</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>12</v>
@@ -5506,7 +5556,7 @@
     </row>
     <row r="99" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B99" s="28" t="s">
         <v>88</v>
@@ -5515,13 +5565,13 @@
         <v>2007</v>
       </c>
       <c r="D99" s="28" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F99" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>12</v>
@@ -5535,7 +5585,7 @@
     </row>
     <row r="100" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>41</v>
@@ -5544,13 +5594,13 @@
         <v>2012</v>
       </c>
       <c r="D100" s="28" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F100" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>12</v>
@@ -5564,7 +5614,7 @@
     </row>
     <row r="101" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>88</v>
@@ -5573,13 +5623,13 @@
         <v>2010</v>
       </c>
       <c r="D101" s="28" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F101" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I101" s="2" t="s">
         <v>12</v>
@@ -5593,7 +5643,7 @@
     </row>
     <row r="102" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>31</v>
@@ -5602,13 +5652,13 @@
         <v>2015</v>
       </c>
       <c r="D102" s="28" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F102" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>12</v>
@@ -5622,7 +5672,7 @@
     </row>
     <row r="103" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B103" s="28" t="s">
         <v>190</v>
@@ -5631,13 +5681,13 @@
         <v>2015</v>
       </c>
       <c r="D103" s="28" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F103" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>12</v>
@@ -5651,7 +5701,7 @@
     </row>
     <row r="104" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B104" s="28" t="s">
         <v>293</v>
@@ -5660,13 +5710,13 @@
         <v>2014</v>
       </c>
       <c r="D104" s="28" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F104" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>12</v>
@@ -5680,22 +5730,22 @@
     </row>
     <row r="105" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C105" s="2">
         <v>2004</v>
       </c>
       <c r="D105" s="28" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F105" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>12</v>
@@ -5709,7 +5759,7 @@
     </row>
     <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B106" s="28" t="s">
         <v>41</v>
@@ -5718,13 +5768,13 @@
         <v>1989</v>
       </c>
       <c r="D106" s="28" t="s">
-        <v>406</v>
+        <v>476</v>
       </c>
       <c r="F106" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>12</v>
@@ -5738,7 +5788,7 @@
     </row>
     <row r="107" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B107" s="28" t="s">
         <v>293</v>
@@ -5753,7 +5803,7 @@
         <v>12</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I107" s="2" t="s">
         <v>12</v>
@@ -5767,7 +5817,7 @@
     </row>
     <row r="108" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B108" s="28" t="s">
         <v>312</v>
@@ -5776,13 +5826,13 @@
         <v>2011</v>
       </c>
       <c r="D108" s="28" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F108" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>12</v>
@@ -5796,7 +5846,7 @@
     </row>
     <row r="109" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B109" s="28" t="s">
         <v>105</v>
@@ -5805,13 +5855,13 @@
         <v>1994</v>
       </c>
       <c r="D109" s="28" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F109" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>12</v>
@@ -5825,7 +5875,7 @@
     </row>
     <row r="110" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B110" s="28" t="s">
         <v>195</v>
@@ -5834,7 +5884,7 @@
         <v>1983</v>
       </c>
       <c r="D110" s="28" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F110" s="23" t="s">
         <v>12</v>
@@ -5846,27 +5896,27 @@
         <v>12</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C111" s="2">
         <v>2010</v>
       </c>
       <c r="D111" s="28" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F111" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>12</v>
@@ -5880,22 +5930,22 @@
     </row>
     <row r="112" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C112" s="2">
         <v>2012</v>
       </c>
       <c r="D112" s="28" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F112" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>12</v>
@@ -5909,22 +5959,22 @@
     </row>
     <row r="113" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B113" s="28" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C113" s="2">
         <v>2013</v>
       </c>
       <c r="D113" s="28" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F113" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>12</v>
@@ -5938,22 +5988,22 @@
     </row>
     <row r="114" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C114" s="2">
         <v>2005</v>
       </c>
       <c r="D114" s="28" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="F114" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>12</v>
@@ -5967,22 +6017,22 @@
     </row>
     <row r="115" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C115" s="2">
         <v>1986</v>
       </c>
       <c r="D115" s="28" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F115" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>12</v>
@@ -5996,7 +6046,7 @@
     </row>
     <row r="116" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B116" s="28" t="s">
         <v>64</v>
@@ -6005,13 +6055,13 @@
         <v>2002</v>
       </c>
       <c r="D116" s="28" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F116" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>12</v>
@@ -6025,22 +6075,22 @@
     </row>
     <row r="117" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B117" s="28" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C117" s="2">
         <v>2004</v>
       </c>
       <c r="D117" s="28" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F117" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>12</v>
@@ -6054,7 +6104,7 @@
     </row>
     <row r="118" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B118" s="28" t="s">
         <v>133</v>
@@ -6063,13 +6113,13 @@
         <v>2022</v>
       </c>
       <c r="D118" s="28" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F118" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>12</v>
@@ -6083,7 +6133,7 @@
     </row>
     <row r="119" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B119" s="28" t="s">
         <v>92</v>
@@ -6092,13 +6142,13 @@
         <v>1994</v>
       </c>
       <c r="D119" s="28" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F119" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>12</v>
@@ -6112,7 +6162,7 @@
     </row>
     <row r="120" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B120" s="28" t="s">
         <v>88</v>
@@ -6121,13 +6171,13 @@
         <v>2011</v>
       </c>
       <c r="D120" s="28" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F120" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G120" s="28" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>12</v>
@@ -6141,7 +6191,7 @@
     </row>
     <row r="121" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B121" s="28" t="s">
         <v>92</v>
@@ -6150,13 +6200,13 @@
         <v>1990</v>
       </c>
       <c r="D121" s="28" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F121" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>12</v>
@@ -6170,7 +6220,7 @@
     </row>
     <row r="122" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B122" s="28" t="s">
         <v>92</v>
@@ -6179,13 +6229,13 @@
         <v>2006</v>
       </c>
       <c r="D122" s="28" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="F122" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="I122" s="2" t="s">
         <v>12</v>
@@ -6199,22 +6249,22 @@
     </row>
     <row r="123" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C123" s="2">
         <v>2012</v>
       </c>
       <c r="D123" s="28" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="F123" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="I123" s="2" t="s">
         <v>12</v>
@@ -6228,7 +6278,7 @@
     </row>
     <row r="124" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B124" s="28" t="s">
         <v>33</v>
@@ -6237,13 +6287,13 @@
         <v>2012</v>
       </c>
       <c r="D124" s="28" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F124" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="I124" s="2" t="s">
         <v>12</v>
@@ -6257,22 +6307,22 @@
     </row>
     <row r="125" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B125" s="28" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C125" s="2">
         <v>2021</v>
       </c>
       <c r="D125" s="28" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="F125" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>12</v>
@@ -6286,7 +6336,7 @@
     </row>
     <row r="126" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B126" s="28" t="s">
         <v>59</v>
@@ -6295,13 +6345,13 @@
         <v>2007</v>
       </c>
       <c r="D126" s="28" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F126" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I126" s="2" t="s">
         <v>12</v>
@@ -6315,7 +6365,7 @@
     </row>
     <row r="127" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B127" s="28" t="s">
         <v>200</v>
@@ -6324,7 +6374,7 @@
         <v>2001</v>
       </c>
       <c r="D127" s="28" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E127" s="12" t="s">
         <v>79</v>
@@ -6333,7 +6383,7 @@
         <v>12</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="I127" s="2" t="s">
         <v>12</v>
@@ -6344,22 +6394,22 @@
     </row>
     <row r="128" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B128" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C128" s="2">
         <v>1970</v>
       </c>
       <c r="D128" s="28" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="F128" s="29" t="s">
         <v>197</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="I128" s="2" t="s">
         <v>12</v>
@@ -6368,6 +6418,70 @@
         <v>12</v>
       </c>
       <c r="K128" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A129" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C129" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="F129" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="H129" s="8"/>
+      <c r="I129" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K129" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A130" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="B130" s="39" t="s">
+        <v>483</v>
+      </c>
+      <c r="C130" s="39">
+        <v>2015</v>
+      </c>
+      <c r="D130" s="39" t="s">
+        <v>484</v>
+      </c>
+      <c r="E130" s="40"/>
+      <c r="F130" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G130" s="39" t="s">
+        <v>481</v>
+      </c>
+      <c r="H130" s="40"/>
+      <c r="I130" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J130" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K130" s="40" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
progress on the todo list
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E495B6-487D-3947-8012-9E5808389576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9FFC52-F5FC-0B47-99BC-7FBABCFA660F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="489">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1616,6 +1616,18 @@
   </si>
   <si>
     <t>Chevin</t>
+  </si>
+  <si>
+    <t>Hibernation energetics of free-ranging little brown bats</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Biology</t>
+  </si>
+  <si>
+    <t>Jonasson &amp; Willis</t>
+  </si>
+  <si>
+    <t>Hibernation in little brown bats (Myotis lucifugus)</t>
   </si>
 </sst>
 </file>
@@ -2403,12 +2415,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P130"/>
+  <dimension ref="A1:P131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A131" sqref="A131"/>
+      <selection pane="bottomLeft" activeCell="K132" sqref="K132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3061,7 +3073,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3103,7 +3115,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6483,6 +6495,35 @@
       </c>
       <c r="K130" s="40" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B131" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="C131" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D131" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="F131" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="I131" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J131" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K131" s="40" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
text done, miss chapter 4
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9FFC52-F5FC-0B47-99BC-7FBABCFA660F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFDD155-C728-214A-9F1C-1E9087BB335F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
+    <workbookView xWindow="29560" yWindow="660" windowWidth="38080" windowHeight="20780" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="495">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1628,6 +1628,24 @@
   </si>
   <si>
     <t>Hibernation in little brown bats (Myotis lucifugus)</t>
+  </si>
+  <si>
+    <t>What Animal Breeding Has Taught Us about Evolution</t>
+  </si>
+  <si>
+    <t>Hill &amp; Kirkpatrick</t>
+  </si>
+  <si>
+    <t>Infinitesimal model</t>
+  </si>
+  <si>
+    <t>Antagonistic pleiotropy and genetic polymorphism: a perspective</t>
+  </si>
+  <si>
+    <t>Hedrick</t>
+  </si>
+  <si>
+    <t>Antagonistic pleiotropy</t>
   </si>
 </sst>
 </file>
@@ -2415,12 +2433,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P131"/>
+  <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="K132" sqref="K132"/>
+      <selection pane="bottomLeft" activeCell="K133" sqref="K133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3073,7 +3091,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3115,7 +3133,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3258,7 +3276,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6524,6 +6542,61 @@
       </c>
       <c r="K131" s="40" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B132" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="C132" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D132" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="F132" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="I132" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J132" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K132" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B133" t="s">
+        <v>492</v>
+      </c>
+      <c r="C133" s="2">
+        <v>1999</v>
+      </c>
+      <c r="D133" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="F133" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="I133" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J133" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K133" s="40" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version for the comps
</commit_message>
<xml_diff>
--- a/research_proposal_biblio.xlsx
+++ b/research_proposal_biblio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinbirot/Desktop/Work/PhD/research/research_proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB605FC-3794-9B44-A6E5-D92804A47FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67486D41-EB89-5F4F-89E1-D1B9DC06CF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29080" windowHeight="16860" xr2:uid="{2464C7AB-A2AF-F64A-8B52-5AEA58554787}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="503">
   <si>
     <t>Paper Title</t>
   </si>
@@ -1658,6 +1658,18 @@
   </si>
   <si>
     <t>Heredity</t>
+  </si>
+  <si>
+    <t>The Hermit Who Inadvertently Shaped Climate-Change Science</t>
+  </si>
+  <si>
+    <t>the atlantic</t>
+  </si>
+  <si>
+    <t>Philippen J. Weston</t>
+  </si>
+  <si>
+    <t>billy barr</t>
   </si>
 </sst>
 </file>
@@ -2445,12 +2457,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FC0888-2B5D-AD42-A2BD-1C837C882783}">
-  <dimension ref="A1:P134"/>
+  <dimension ref="A1:P135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+      <selection pane="bottomLeft" activeCell="K135" sqref="K135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3103,7 +3115,7 @@
       </c>
       <c r="N19" s="14">
         <f>N20+N26</f>
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3145,7 +3157,7 @@
       </c>
       <c r="N20" s="14">
         <f>COUNTIF(J:J, "yes")</f>
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3222,7 +3234,7 @@
       </c>
       <c r="N22" s="21">
         <f>COUNTIF(F:F, "no")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3288,7 +3300,7 @@
       </c>
       <c r="N24" s="19">
         <f>COUNTIF(K:K, "yes")</f>
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6640,6 +6652,35 @@
         <v>12</v>
       </c>
       <c r="K134" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A135" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B135" t="s">
+        <v>500</v>
+      </c>
+      <c r="C135" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D135" s="28" t="s">
+        <v>501</v>
+      </c>
+      <c r="F135" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="I135" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="J135" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K135" s="40" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>